<commit_message>
solves questions from sheet
</commit_message>
<xml_diff>
--- a/DSA Sheet.xlsx
+++ b/DSA Sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d8cfd04c6706e178/Desktop/myDSA/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="12" documentId="11_3A057C0BE92A3E6736330E251CF58AC5C01E7902" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{97A01B40-A9A4-4280-9CD0-830ECC8223AA}"/>
+  <xr:revisionPtr revIDLastSave="48" documentId="11_3A057C0BE92A3E6736330E251CF58AC5C01E7902" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1783FD76-E9BB-4E18-ADF0-4FB8C412EB45}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="401" uniqueCount="361">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="401" uniqueCount="362">
   <si>
     <t>Arrays</t>
   </si>
@@ -1147,9 +1147,6 @@
     <t>LEETCODE CODING SHEET</t>
   </si>
   <si>
-    <t>BINARY TREES</t>
-  </si>
-  <si>
     <t>https://leetcode.com/problems/binary-tree-preorder-traversal/</t>
   </si>
   <si>
@@ -1169,6 +1166,12 @@
   </si>
   <si>
     <t>https://leetcode.com/problems/count-complete-tree-nodes/</t>
+  </si>
+  <si>
+    <t>heap problem-solved with using the static int from the previous func by pass by address.</t>
+  </si>
+  <si>
+    <t>We need to do it using stack but change the implementations at few points.</t>
   </si>
 </sst>
 </file>
@@ -1275,7 +1278,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1300,6 +1303,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -1314,7 +1323,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1346,6 +1355,9 @@
     <xf numFmtId="0" fontId="14" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1565,10 +1577,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="B1:C441"/>
+  <dimension ref="B1:D446"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A421" workbookViewId="0">
-      <selection activeCell="B444" sqref="B444"/>
+    <sheetView tabSelected="1" topLeftCell="A188" workbookViewId="0">
+      <selection activeCell="B452" sqref="B452"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1577,273 +1589,273 @@
     <col min="3" max="3" width="62.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B1" s="1"/>
     </row>
-    <row r="2" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B2" s="13" t="s">
         <v>352</v>
       </c>
     </row>
-    <row r="3" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B3" s="2"/>
     </row>
-    <row r="5" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B6" s="4" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B7" s="5" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B8" s="5" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B9" s="5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B10" s="5" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B11" s="5" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B12" s="6" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="13" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B13" s="6" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="14" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B14" s="6" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="15" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B15" s="6" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="16" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B16" s="6" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B17" s="6" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B18" s="6" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="20" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B20" s="4" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="21" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B21" s="5" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="22" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B22" s="6" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="23" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B23" s="6" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="24" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B24" s="6" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="25" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B25" s="6" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="26" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B26" s="6" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="27" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B27" s="6" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="28" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B28" s="6" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="29" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B29" s="6" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="30" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B30" s="6" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="31" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B31" s="6" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="32" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B32" s="6" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="33" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B33" s="6" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="34" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B34" s="6" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="35" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B35" s="6" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="36" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B36" s="6" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="37" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B37" s="5" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="38" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B38" s="5" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="39" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B39" s="5" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="40" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B40" s="5" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="41" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B41" s="6" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="42" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B42" s="6" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="43" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B43" s="6" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="44" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B44" s="6" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="45" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B45" s="6" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="46" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B46" s="6" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="48" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B48" s="4" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="49" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B49" s="14" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="50" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B50" s="6" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="51" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B51" s="6" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="52" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B52" s="6" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="53" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B53" s="6" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="55" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B55" s="3" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="56" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B56" s="4" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="57" spans="2:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B57" s="5" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="58" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="58" spans="2:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B58" s="6" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="59" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="59" spans="2:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B59" s="6" t="s">
         <v>50</v>
       </c>
@@ -1851,1740 +1863,1765 @@
         <v>51</v>
       </c>
     </row>
-    <row r="60" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="60" spans="2:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B60" s="5" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="62" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="62" spans="2:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B62" s="4" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="63" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="63" spans="2:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B63" s="6" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="64" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="64" spans="2:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B64" s="6" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="65" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="65" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B65" s="6" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="66" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="66" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B66" s="6" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="67" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="67" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B67" s="6" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="68" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="68" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B68" s="6" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="69" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="69" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B69" s="6" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="70" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="70" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B70" s="6" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="71" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="71" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B71" s="6" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="72" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="72" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B72" s="6" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="73" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="73" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B73" s="6" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="74" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="74" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B74" s="6" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="75" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="75" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B75" s="6" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="76" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="76" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B76" s="6" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="77" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="77" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B77" s="6" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="79" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="79" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B79" s="4" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="80" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="80" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B80" s="6" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="81" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="81" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B81" s="6" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="82" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="82" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B82" s="6" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="83" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="83" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B83" s="6" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="84" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="84" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B84" s="6" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="85" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="85" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B85" s="6" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="86" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="86" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B86" s="6" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="87" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="87" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B87" s="6" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="88" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="88" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B88" s="6" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="89" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="89" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B89" s="6" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="90" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="90" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B90" s="6" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="91" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="91" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B91" s="6" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="92" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="92" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B92" s="6" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="93" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="93" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B93" s="6" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="94" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="94" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B94" s="6" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="96" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="96" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B96" s="3" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="97" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="97" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B97" s="4" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="98" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="98" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B98" s="6" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="99" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="99" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B99" s="6" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="100" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="100" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B100" s="6" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="101" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="101" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B101" s="6" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="102" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="102" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B102" s="6" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="104" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="104" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B104" s="4" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="105" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="105" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B105" s="6" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="106" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="106" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B106" s="6" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="107" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="107" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B107" s="6" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="108" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="108" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B108" s="6" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="109" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="109" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B109" s="6" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="110" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="110" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B110" s="6" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="111" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="111" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B111" s="6" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="112" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="112" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B112" s="5" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="113" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="113" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B113" s="6" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="114" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="114" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B114" s="6" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="115" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="115" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B115" s="6" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="117" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="117" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B117" s="4" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="118" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="118" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B118" s="5" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="119" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="119" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B119" s="5" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="120" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="120" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B120" s="6" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="121" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="121" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B121" s="6" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="122" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="122" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B122" s="6" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="123" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="123" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B123" s="6" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="124" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="124" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B124" s="6" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="126" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="126" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B126" s="3" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="127" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="127" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B127" s="4" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="128" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="128" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B128" s="5" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="129" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="129" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B129" s="6" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="130" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="130" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B130" s="5" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="131" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="131" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B131" s="5" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="132" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="132" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B132" s="5" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="133" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="133" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B133" s="5" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="134" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="134" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B134" s="5" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="135" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="135" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B135" s="5" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="136" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="136" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B136" s="5" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="138" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="138" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B138" s="4" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="139" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="139" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B139" s="5" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="140" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="140" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B140" s="5" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="141" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="141" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B141" s="5" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="142" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="142" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B142" s="5" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="143" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="143" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B143" s="5" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="144" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="144" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B144" s="5" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="145" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="145" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B145" s="5" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="147" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="147" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B147" s="4" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="148" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="148" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B148" s="6" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="149" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="149" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B149" s="6" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="150" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="150" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B150" s="6" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="151" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="151" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B151" s="6" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="153" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="153" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B153" s="3" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="154" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="154" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B154" s="4" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="155" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="155" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B155" s="7" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="157" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="157" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B157" s="4" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="158" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="158" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B158" s="5" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="159" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="159" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B159" s="5" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="160" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="160" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B160" s="5" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="161" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="161" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B161" s="5" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="162" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="162" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B162" s="5" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="163" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="163" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B163" s="5" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="164" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="164" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B164" s="5" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="165" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="165" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B165" s="6" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="167" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="167" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B167" s="4" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="168" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="168" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B168" s="5" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="169" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="169" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B169" s="6" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="170" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="170" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B170" s="5" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="172" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="172" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B172" s="3" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="173" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="173" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B173" s="4" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="174" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="174" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B174" s="5" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="175" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="175" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B175" s="5" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="176" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="176" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B176" s="5" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="177" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="177" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B177" s="5" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="178" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="178" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B178" s="5" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="179" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="179" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B179" s="5" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="180" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="180" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B180" s="5" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="181" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="181" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B181" s="8" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="182" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="182" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B182" s="5" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="184" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="184" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B184" s="4" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="185" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="185" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B185" s="5" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="186" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="186" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B186" s="5" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="187" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="187" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B187" s="5" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="188" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="188" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B188" s="5" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="189" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="189" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B189" s="5" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="190" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="190" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B190" s="5" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="191" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="191" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B191" s="5" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="192" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="192" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B192" s="5" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="194" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="194" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B194" s="3" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="195" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="195" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B195" s="4" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="196" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="196" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B196" s="6" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="197" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="197" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B197" s="6" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="198" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="198" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B198" s="5" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="199" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="199" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B199" s="6" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="200" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="200" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B200" s="5" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="201" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="201" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B201" s="5" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="202" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="202" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B202" s="6" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="203" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="203" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B203" s="5" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="204" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="204" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B204" s="6" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="205" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="205" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B205" s="5" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="206" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="206" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B206" s="6" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="207" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="207" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B207" s="6" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="208" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="208" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B208" s="5" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="209" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="209" spans="2:4" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B209" s="6" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="210" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="210" spans="2:4" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B210" s="5" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="211" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="211" spans="2:4" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B211" s="15" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="213" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B213" s="4" t="s">
+    <row r="212" spans="2:4" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B212" s="17" t="s">
+        <v>353</v>
+      </c>
+      <c r="C212" s="16" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="213" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B213" s="17" t="s">
+        <v>355</v>
+      </c>
+      <c r="C213" s="18" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="214" spans="2:4" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B214" s="17" t="s">
+        <v>356</v>
+      </c>
+      <c r="C214" s="16" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="215" spans="2:4" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="D215" s="16"/>
+    </row>
+    <row r="216" spans="2:4" ht="13.2" x14ac:dyDescent="0.25"/>
+    <row r="217" spans="2:4" ht="13.2" x14ac:dyDescent="0.25"/>
+    <row r="218" spans="2:4" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B218" s="4" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="214" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B214" s="5" t="s">
+    <row r="219" spans="2:4" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B219" s="5" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="215" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B215" s="6" t="s">
+    <row r="220" spans="2:4" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B220" s="6" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="216" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B216" s="6" t="s">
+    <row r="221" spans="2:4" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B221" s="6" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="217" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B217" s="6" t="s">
+    <row r="222" spans="2:4" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B222" s="6" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="218" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B218" s="6" t="s">
+    <row r="223" spans="2:4" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B223" s="6" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="219" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B219" s="6" t="s">
+    <row r="224" spans="2:4" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B224" s="6" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="220" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B220" s="6" t="s">
+    <row r="225" spans="2:3" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B225" s="6" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="221" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B221" s="6" t="s">
+    <row r="226" spans="2:3" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B226" s="22" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="222" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B222" s="6" t="s">
+    <row r="227" spans="2:3" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B227" s="6" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="223" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B223" s="6" t="s">
+    <row r="228" spans="2:3" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B228" s="6" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="224" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B224" s="6" t="s">
+    <row r="229" spans="2:3" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B229" s="6" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="225" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B225" s="6" t="s">
+    <row r="230" spans="2:3" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B230" s="6" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="226" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B226" s="6" t="s">
+    <row r="231" spans="2:3" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B231" s="6" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="227" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B227" s="6" t="s">
+    <row r="232" spans="2:3" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B232" s="6" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="228" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B228" s="6" t="s">
+    <row r="233" spans="2:3" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B233" s="6" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="229" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B229" s="6" t="s">
+    <row r="234" spans="2:3" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B234" s="6" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="230" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B230" s="6" t="s">
+    <row r="235" spans="2:3" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B235" s="6" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="231" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B231" s="6" t="s">
+    <row r="236" spans="2:3" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B236" s="6" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="233" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B233" s="4" t="s">
+    <row r="237" spans="2:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B237" s="21" t="s">
+        <v>357</v>
+      </c>
+      <c r="C237" s="16" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="238" spans="2:3" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B238" s="21" t="s">
+        <v>358</v>
+      </c>
+      <c r="C238" s="16" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="239" spans="2:3" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B239" s="23" t="s">
+        <v>184</v>
+      </c>
+      <c r="C239" s="16" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="240" spans="2:3" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B240" s="17" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="241" spans="2:2" ht="13.2" x14ac:dyDescent="0.25"/>
+    <row r="242" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B242" s="4" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="234" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B234" s="6" t="s">
+    <row r="243" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B243" s="6" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="235" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B235" s="6" t="s">
+    <row r="244" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B244" s="6" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="236" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B236" s="5" t="s">
+    <row r="245" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B245" s="5" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="237" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B237" s="6" t="s">
+    <row r="246" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B246" s="6" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="238" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B238" s="6" t="s">
+    <row r="247" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B247" s="6" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="239" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B239" s="6" t="s">
+    <row r="248" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B248" s="6" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="240" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B240" s="6" t="s">
+    <row r="249" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B249" s="6" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="242" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B242" s="3" t="s">
+    <row r="250" spans="2:2" ht="13.2" x14ac:dyDescent="0.25"/>
+    <row r="251" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B251" s="3" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="243" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B243" s="4" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="244" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B244" s="6" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="245" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B245" s="6" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="246" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B246" s="9"/>
-    </row>
-    <row r="247" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B247" s="4" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="248" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B248" s="6" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="249" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B249" s="6" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="251" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B251" s="3" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="252" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="252" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B252" s="4" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="253" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B253" s="5" t="s">
+    <row r="253" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B253" s="6" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="254" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B254" s="6" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="255" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B255" s="9"/>
+    </row>
+    <row r="256" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B256" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="257" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B257" s="6" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="258" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B258" s="6" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="259" spans="2:2" ht="13.2" x14ac:dyDescent="0.25"/>
+    <row r="260" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B260" s="3" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="261" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B261" s="4" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="262" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B262" s="5" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="254" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B254" s="6" t="s">
+    <row r="263" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B263" s="6" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="255" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B255" s="6" t="s">
+    <row r="264" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B264" s="6" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="256" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B256" s="6" t="s">
+    <row r="265" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B265" s="6" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="258" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B258" s="4" t="s">
+    <row r="266" spans="2:2" ht="13.2" x14ac:dyDescent="0.25"/>
+    <row r="267" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B267" s="4" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="259" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B259" s="6" t="s">
+    <row r="268" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B268" s="6" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="260" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B260" s="6" t="s">
+    <row r="269" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B269" s="6" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="261" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B261" s="6" t="s">
+    <row r="270" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B270" s="6" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="262" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B262" s="6" t="s">
+    <row r="271" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B271" s="6" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="263" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B263" s="6" t="s">
+    <row r="272" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B272" s="6" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="264" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B264" s="6" t="s">
+    <row r="273" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B273" s="6" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="265" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B265" s="6" t="s">
+    <row r="274" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B274" s="6" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="266" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B266" s="6" t="s">
+    <row r="275" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B275" s="6" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="267" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B267" s="6" t="s">
+    <row r="276" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B276" s="6" t="s">
         <v>220</v>
       </c>
     </row>
-    <row r="269" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B269" s="4" t="s">
+    <row r="277" spans="2:2" ht="13.2" x14ac:dyDescent="0.25"/>
+    <row r="278" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B278" s="4" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="270" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B270" s="6" t="s">
+    <row r="279" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B279" s="6" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="271" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B271" s="6" t="s">
+    <row r="280" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B280" s="6" t="s">
         <v>222</v>
       </c>
     </row>
-    <row r="272" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B272" s="6" t="s">
+    <row r="281" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B281" s="6" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="273" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B273" s="6" t="s">
+    <row r="282" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B282" s="6" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="274" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B274" s="6" t="s">
+    <row r="283" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B283" s="6" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="276" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B276" s="3" t="s">
+    <row r="284" spans="2:2" ht="13.2" x14ac:dyDescent="0.25"/>
+    <row r="285" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B285" s="3" t="s">
         <v>226</v>
       </c>
     </row>
-    <row r="277" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B277" s="4" t="s">
+    <row r="286" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B286" s="4" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="278" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B278" s="6" t="s">
+    <row r="287" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B287" s="6" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="279" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B279" s="6" t="s">
+    <row r="288" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B288" s="6" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="280" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B280" s="6" t="s">
+    <row r="289" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B289" s="6" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="281" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B281" s="6" t="s">
+    <row r="290" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B290" s="6" t="s">
         <v>230</v>
       </c>
     </row>
-    <row r="282" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B282" s="5" t="s">
+    <row r="291" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B291" s="5" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="284" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B284" s="4" t="s">
+    <row r="292" spans="2:2" ht="13.2" x14ac:dyDescent="0.25"/>
+    <row r="293" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B293" s="4" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="285" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B285" s="6" t="s">
+    <row r="294" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B294" s="6" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="286" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B286" s="6" t="s">
+    <row r="295" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B295" s="6" t="s">
         <v>233</v>
       </c>
     </row>
-    <row r="287" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B287" s="6" t="s">
+    <row r="296" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B296" s="6" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="288" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B288" s="6" t="s">
+    <row r="297" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B297" s="6" t="s">
         <v>235</v>
       </c>
     </row>
-    <row r="290" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B290" s="3" t="s">
+    <row r="298" spans="2:2" ht="13.2" x14ac:dyDescent="0.25"/>
+    <row r="299" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B299" s="3" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="291" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B291" s="4" t="s">
+    <row r="300" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B300" s="4" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="292" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B292" s="6" t="s">
+    <row r="301" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B301" s="6" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="293" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B293" s="6" t="s">
+    <row r="302" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B302" s="6" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="294" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B294" s="6" t="s">
+    <row r="303" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B303" s="6" t="s">
         <v>240</v>
       </c>
     </row>
-    <row r="295" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B295" s="6" t="s">
+    <row r="304" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B304" s="6" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="296" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B296" s="6" t="s">
+    <row r="305" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B305" s="6" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="298" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B298" s="3" t="s">
+    <row r="306" spans="2:2" ht="13.2" x14ac:dyDescent="0.25"/>
+    <row r="307" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B307" s="3" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="299" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B299" s="4" t="s">
+    <row r="308" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B308" s="4" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="300" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B300" s="6" t="s">
+    <row r="309" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B309" s="6" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="301" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B301" s="6" t="s">
+    <row r="310" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B310" s="6" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="302" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B302" s="6" t="s">
+    <row r="311" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B311" s="6" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="303" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B303" s="6" t="s">
+    <row r="312" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B312" s="6" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="304" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B304" s="6" t="s">
+    <row r="313" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B313" s="6" t="s">
         <v>248</v>
       </c>
     </row>
-    <row r="305" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B305" s="6" t="s">
+    <row r="314" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B314" s="6" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="307" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B307" s="4" t="s">
+    <row r="315" spans="2:2" ht="13.2" x14ac:dyDescent="0.25"/>
+    <row r="316" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B316" s="4" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="308" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B308" s="5" t="s">
+    <row r="317" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B317" s="5" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="309" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B309" s="6" t="s">
+    <row r="318" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B318" s="6" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="310" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B310" s="6" t="s">
+    <row r="319" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B319" s="6" t="s">
         <v>252</v>
       </c>
     </row>
-    <row r="311" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B311" s="6" t="s">
+    <row r="320" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B320" s="6" t="s">
         <v>253</v>
       </c>
     </row>
-    <row r="313" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B313" s="3" t="s">
+    <row r="321" spans="2:3" ht="13.2" x14ac:dyDescent="0.25"/>
+    <row r="322" spans="2:3" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B322" s="3" t="s">
         <v>254</v>
       </c>
     </row>
-    <row r="314" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B314" s="4" t="s">
+    <row r="323" spans="2:3" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B323" s="4" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="315" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B315" s="6" t="s">
+    <row r="324" spans="2:3" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B324" s="6" t="s">
         <v>255</v>
       </c>
     </row>
-    <row r="316" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B316" s="6" t="s">
+    <row r="325" spans="2:3" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B325" s="6" t="s">
         <v>256</v>
       </c>
-      <c r="C316" s="5" t="s">
+      <c r="C325" s="5" t="s">
         <v>257</v>
       </c>
     </row>
-    <row r="317" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B317" s="6" t="s">
+    <row r="326" spans="2:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B326" s="6" t="s">
         <v>258</v>
       </c>
     </row>
-    <row r="318" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B318" s="5" t="s">
+    <row r="327" spans="2:3" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B327" s="5" t="s">
         <v>259</v>
       </c>
     </row>
-    <row r="319" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B319" s="20" t="s">
+    <row r="328" spans="2:3" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B328" s="20" t="s">
         <v>260</v>
       </c>
-      <c r="C319" s="8" t="s">
+      <c r="C328" s="8" t="s">
         <v>261</v>
       </c>
     </row>
-    <row r="320" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B320" s="5" t="s">
+    <row r="329" spans="2:3" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B329" s="5" t="s">
         <v>262</v>
       </c>
     </row>
-    <row r="322" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B322" s="4" t="s">
+    <row r="330" spans="2:3" ht="13.2" x14ac:dyDescent="0.25"/>
+    <row r="331" spans="2:3" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B331" s="4" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="323" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B323" s="5" t="s">
+    <row r="332" spans="2:3" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B332" s="5" t="s">
         <v>263</v>
       </c>
     </row>
-    <row r="324" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B324" s="6" t="s">
+    <row r="333" spans="2:3" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B333" s="6" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="325" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B325" s="6" t="s">
+    <row r="334" spans="2:3" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B334" s="6" t="s">
         <v>265</v>
       </c>
     </row>
-    <row r="326" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B326" s="6" t="s">
+    <row r="335" spans="2:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B335" s="6" t="s">
         <v>266</v>
       </c>
     </row>
-    <row r="327" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B327" s="5" t="s">
+    <row r="336" spans="2:3" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B336" s="5" t="s">
         <v>267</v>
       </c>
     </row>
-    <row r="328" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B328" s="6" t="s">
+    <row r="337" spans="2:3" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B337" s="6" t="s">
         <v>268</v>
       </c>
-      <c r="C328" s="6" t="s">
+      <c r="C337" s="6" t="s">
         <v>269</v>
       </c>
     </row>
-    <row r="329" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B329" s="5" t="s">
+    <row r="338" spans="2:3" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B338" s="5" t="s">
         <v>270</v>
       </c>
     </row>
-    <row r="331" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B331" s="3" t="s">
+    <row r="339" spans="2:3" ht="13.2" x14ac:dyDescent="0.25"/>
+    <row r="340" spans="2:3" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B340" s="3" t="s">
         <v>271</v>
       </c>
     </row>
-    <row r="332" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B332" s="4" t="s">
+    <row r="341" spans="2:3" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B341" s="4" t="s">
         <v>272</v>
       </c>
     </row>
-    <row r="333" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B333" s="5" t="s">
+    <row r="342" spans="2:3" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B342" s="5" t="s">
         <v>273</v>
       </c>
     </row>
-    <row r="334" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B334" s="6" t="s">
+    <row r="343" spans="2:3" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B343" s="6" t="s">
         <v>274</v>
       </c>
     </row>
-    <row r="335" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B335" s="6" t="s">
+    <row r="344" spans="2:3" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B344" s="6" t="s">
         <v>275</v>
       </c>
     </row>
-    <row r="336" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B336" s="6" t="s">
+    <row r="345" spans="2:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B345" s="6" t="s">
         <v>276</v>
       </c>
     </row>
-    <row r="337" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B337" s="6" t="s">
+    <row r="346" spans="2:3" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B346" s="6" t="s">
         <v>277</v>
       </c>
     </row>
-    <row r="338" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B338" s="5" t="s">
+    <row r="347" spans="2:3" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B347" s="5" t="s">
         <v>278</v>
       </c>
     </row>
-    <row r="339" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B339" s="6" t="s">
+    <row r="348" spans="2:3" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B348" s="6" t="s">
         <v>279</v>
       </c>
     </row>
-    <row r="341" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B341" s="3" t="s">
+    <row r="349" spans="2:3" ht="13.2" x14ac:dyDescent="0.25"/>
+    <row r="350" spans="2:3" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B350" s="3" t="s">
         <v>280</v>
       </c>
     </row>
-    <row r="342" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B342" s="4" t="s">
+    <row r="351" spans="2:3" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B351" s="4" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="343" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B343" s="5" t="s">
+    <row r="352" spans="2:3" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B352" s="5" t="s">
         <v>281</v>
       </c>
     </row>
-    <row r="344" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B344" s="6" t="s">
+    <row r="353" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B353" s="6" t="s">
         <v>282</v>
       </c>
     </row>
-    <row r="345" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B345" s="10"/>
-    </row>
-    <row r="346" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B346" s="4" t="s">
+    <row r="354" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B354" s="10"/>
+    </row>
+    <row r="355" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B355" s="4" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="347" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B347" s="6" t="s">
+    <row r="356" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B356" s="6" t="s">
         <v>283</v>
       </c>
     </row>
-    <row r="348" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B348" s="6" t="s">
+    <row r="357" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B357" s="6" t="s">
         <v>284</v>
       </c>
     </row>
-    <row r="349" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B349" s="6" t="s">
+    <row r="358" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B358" s="6" t="s">
         <v>285</v>
       </c>
     </row>
-    <row r="350" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B350" s="6" t="s">
+    <row r="359" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B359" s="6" t="s">
         <v>286</v>
       </c>
     </row>
-    <row r="351" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B351" s="6" t="s">
+    <row r="360" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B360" s="6" t="s">
         <v>287</v>
       </c>
     </row>
-    <row r="352" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B352" s="6" t="s">
+    <row r="361" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B361" s="6" t="s">
         <v>288</v>
       </c>
     </row>
-    <row r="353" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B353" s="6" t="s">
+    <row r="362" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B362" s="6" t="s">
         <v>289</v>
       </c>
     </row>
-    <row r="354" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B354" s="6" t="s">
+    <row r="363" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B363" s="6" t="s">
         <v>290</v>
       </c>
     </row>
-    <row r="355" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B355" s="6" t="s">
+    <row r="364" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B364" s="6" t="s">
         <v>291</v>
       </c>
     </row>
-    <row r="356" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B356" s="6" t="s">
+    <row r="365" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B365" s="6" t="s">
         <v>292</v>
       </c>
     </row>
-    <row r="357" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B357" s="6" t="s">
+    <row r="366" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B366" s="6" t="s">
         <v>293</v>
       </c>
     </row>
-    <row r="358" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B358" s="5" t="s">
+    <row r="367" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B367" s="5" t="s">
         <v>294</v>
       </c>
     </row>
-    <row r="359" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B359" s="6" t="s">
+    <row r="368" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B368" s="6" t="s">
         <v>295</v>
       </c>
     </row>
-    <row r="360" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B360" s="6" t="s">
+    <row r="369" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B369" s="6" t="s">
         <v>296</v>
       </c>
     </row>
-    <row r="362" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B362" s="3" t="s">
+    <row r="370" spans="2:2" ht="13.2" x14ac:dyDescent="0.25"/>
+    <row r="371" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B371" s="3" t="s">
         <v>297</v>
       </c>
     </row>
-    <row r="363" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B363" s="6" t="s">
+    <row r="372" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B372" s="6" t="s">
         <v>298</v>
       </c>
     </row>
-    <row r="365" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B365" s="3" t="s">
+    <row r="373" spans="2:2" ht="13.2" x14ac:dyDescent="0.25"/>
+    <row r="374" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B374" s="3" t="s">
         <v>299</v>
       </c>
     </row>
-    <row r="366" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B366" s="11" t="s">
+    <row r="375" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B375" s="11" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="367" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B367" s="6" t="s">
+    <row r="376" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B376" s="6" t="s">
         <v>300</v>
       </c>
     </row>
-    <row r="368" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B368" s="6" t="s">
+    <row r="377" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B377" s="6" t="s">
         <v>301</v>
       </c>
     </row>
-    <row r="369" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B369" s="6" t="s">
+    <row r="378" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B378" s="6" t="s">
         <v>302</v>
       </c>
     </row>
-    <row r="370" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B370" s="6" t="s">
+    <row r="379" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B379" s="6" t="s">
         <v>303</v>
       </c>
     </row>
-    <row r="371" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B371" s="6" t="s">
+    <row r="380" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B380" s="6" t="s">
         <v>304</v>
       </c>
     </row>
-    <row r="372" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B372" s="6" t="s">
+    <row r="381" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B381" s="6" t="s">
         <v>305</v>
       </c>
     </row>
-    <row r="373" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B373" s="6" t="s">
+    <row r="382" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B382" s="6" t="s">
         <v>306</v>
       </c>
     </row>
-    <row r="374" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B374" s="6" t="s">
+    <row r="383" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B383" s="6" t="s">
         <v>307</v>
       </c>
     </row>
-    <row r="375" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B375" s="6" t="s">
+    <row r="384" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B384" s="6" t="s">
         <v>308</v>
       </c>
     </row>
-    <row r="376" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B376" s="6" t="s">
+    <row r="385" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B385" s="6" t="s">
         <v>309</v>
       </c>
     </row>
-    <row r="378" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B378" s="4" t="s">
+    <row r="386" spans="2:2" ht="13.2" x14ac:dyDescent="0.25"/>
+    <row r="387" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B387" s="4" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="379" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B379" s="6" t="s">
+    <row r="388" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B388" s="6" t="s">
         <v>310</v>
       </c>
     </row>
-    <row r="380" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B380" s="6" t="s">
+    <row r="389" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B389" s="6" t="s">
         <v>311</v>
       </c>
     </row>
-    <row r="381" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B381" s="6" t="s">
+    <row r="390" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B390" s="6" t="s">
         <v>312</v>
       </c>
     </row>
-    <row r="382" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B382" s="6" t="s">
+    <row r="391" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B391" s="6" t="s">
         <v>313</v>
       </c>
     </row>
-    <row r="383" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B383" s="5" t="s">
+    <row r="392" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B392" s="5" t="s">
         <v>314</v>
       </c>
     </row>
-    <row r="384" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B384" s="5" t="s">
+    <row r="393" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B393" s="5" t="s">
         <v>315</v>
       </c>
     </row>
-    <row r="385" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B385" s="6" t="s">
+    <row r="394" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B394" s="6" t="s">
         <v>316</v>
       </c>
     </row>
-    <row r="386" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B386" s="5" t="s">
+    <row r="395" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B395" s="5" t="s">
         <v>317</v>
       </c>
     </row>
-    <row r="387" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B387" s="6" t="s">
+    <row r="396" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B396" s="6" t="s">
         <v>318</v>
       </c>
     </row>
-    <row r="388" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B388" s="6" t="s">
+    <row r="397" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B397" s="6" t="s">
         <v>319</v>
       </c>
     </row>
-    <row r="389" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B389" s="6" t="s">
+    <row r="398" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B398" s="6" t="s">
         <v>320</v>
       </c>
     </row>
-    <row r="390" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B390" s="6" t="s">
+    <row r="399" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B399" s="6" t="s">
         <v>321</v>
       </c>
     </row>
-    <row r="391" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B391" s="6" t="s">
+    <row r="400" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B400" s="6" t="s">
         <v>322</v>
       </c>
     </row>
-    <row r="393" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B393" s="4" t="s">
+    <row r="402" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B402" s="4" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="394" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B394" s="5" t="s">
+    <row r="403" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B403" s="5" t="s">
         <v>323</v>
       </c>
     </row>
-    <row r="395" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B395" s="6" t="s">
+    <row r="404" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B404" s="6" t="s">
         <v>324</v>
       </c>
     </row>
-    <row r="397" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B397" s="3" t="s">
+    <row r="405" spans="2:2" ht="13.2" x14ac:dyDescent="0.25"/>
+    <row r="406" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B406" s="3" t="s">
         <v>325</v>
       </c>
     </row>
-    <row r="398" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B398" s="4" t="s">
+    <row r="407" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B407" s="4" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="399" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B399" s="6" t="s">
+    <row r="408" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B408" s="6" t="s">
         <v>326</v>
       </c>
     </row>
-    <row r="400" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B400" s="6" t="s">
+    <row r="409" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B409" s="6" t="s">
         <v>327</v>
       </c>
     </row>
-    <row r="401" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B401" s="6" t="s">
+    <row r="410" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B410" s="6" t="s">
         <v>328</v>
       </c>
     </row>
-    <row r="402" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B402" s="6" t="s">
+    <row r="411" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B411" s="6" t="s">
         <v>329</v>
       </c>
     </row>
-    <row r="403" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B403" s="6" t="s">
+    <row r="412" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B412" s="6" t="s">
         <v>330</v>
       </c>
     </row>
-    <row r="404" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B404" s="6" t="s">
+    <row r="413" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B413" s="6" t="s">
         <v>331</v>
       </c>
     </row>
-    <row r="405" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B405" s="6" t="s">
+    <row r="414" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B414" s="6" t="s">
         <v>332</v>
       </c>
     </row>
-    <row r="406" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B406" s="6" t="s">
+    <row r="415" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B415" s="6" t="s">
         <v>333</v>
       </c>
     </row>
-    <row r="408" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B408" s="4" t="s">
+    <row r="416" spans="2:2" ht="13.2" x14ac:dyDescent="0.25"/>
+    <row r="417" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B417" s="4" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="409" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B409" s="6" t="s">
+    <row r="418" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B418" s="6" t="s">
         <v>323</v>
       </c>
     </row>
-    <row r="410" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B410" s="6" t="s">
+    <row r="419" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B419" s="6" t="s">
         <v>334</v>
       </c>
     </row>
-    <row r="411" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B411" s="6" t="s">
+    <row r="420" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B420" s="6" t="s">
         <v>335</v>
       </c>
     </row>
-    <row r="412" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B412" s="6" t="s">
+    <row r="421" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B421" s="6" t="s">
         <v>336</v>
       </c>
     </row>
-    <row r="413" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B413" s="5" t="s">
+    <row r="422" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B422" s="5" t="s">
         <v>337</v>
       </c>
     </row>
-    <row r="414" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B414" s="6" t="s">
+    <row r="423" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B423" s="6" t="s">
         <v>338</v>
       </c>
     </row>
-    <row r="415" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B415" s="6" t="s">
+    <row r="424" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B424" s="6" t="s">
         <v>339</v>
       </c>
     </row>
-    <row r="416" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B416" s="6" t="s">
+    <row r="425" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B425" s="6" t="s">
         <v>340</v>
       </c>
     </row>
-    <row r="417" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B417" s="6" t="s">
+    <row r="426" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B426" s="6" t="s">
         <v>341</v>
       </c>
     </row>
-    <row r="419" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B419" s="3" t="s">
+    <row r="427" spans="2:2" ht="13.2" x14ac:dyDescent="0.25"/>
+    <row r="428" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B428" s="3" t="s">
         <v>342</v>
       </c>
     </row>
-    <row r="420" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B420" s="4" t="s">
+    <row r="429" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B429" s="4" t="s">
         <v>343</v>
       </c>
     </row>
-    <row r="421" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B421" s="6" t="s">
+    <row r="430" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B430" s="6" t="s">
         <v>344</v>
       </c>
     </row>
-    <row r="422" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B422" s="6" t="s">
+    <row r="431" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B431" s="6" t="s">
         <v>345</v>
       </c>
     </row>
-    <row r="423" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B423" s="6" t="s">
+    <row r="432" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B432" s="6" t="s">
         <v>346</v>
       </c>
     </row>
-    <row r="424" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B424" s="12" t="s">
+    <row r="433" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B433" s="12" t="s">
         <v>347</v>
       </c>
     </row>
-    <row r="425" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B425" s="4"/>
-    </row>
-    <row r="426" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B426" s="3" t="s">
+    <row r="434" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B434" s="4"/>
+    </row>
+    <row r="435" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B435" s="3" t="s">
         <v>348</v>
       </c>
     </row>
-    <row r="427" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B427" s="5" t="s">
+    <row r="436" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B436" s="5" t="s">
         <v>349</v>
       </c>
     </row>
-    <row r="428" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B428" s="3" t="s">
+    <row r="437" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B437" s="3" t="s">
         <v>350</v>
       </c>
     </row>
-    <row r="429" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B429" s="5" t="s">
+    <row r="438" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B438" s="5" t="s">
         <v>351</v>
       </c>
     </row>
-    <row r="431" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B431" s="3" t="s">
-        <v>353</v>
-      </c>
-    </row>
-    <row r="432" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B432" s="19" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="433" spans="2:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B433" s="17" t="s">
-        <v>354</v>
-      </c>
-      <c r="C433" s="16" t="s">
-        <v>355</v>
-      </c>
-    </row>
-    <row r="434" spans="2:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B434" s="17" t="s">
-        <v>356</v>
-      </c>
-      <c r="C434" s="18" t="s">
-        <v>355</v>
-      </c>
-    </row>
-    <row r="435" spans="2:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B435" s="17" t="s">
-        <v>357</v>
-      </c>
-      <c r="C435" s="16" t="s">
-        <v>355</v>
-      </c>
-    </row>
-    <row r="436" spans="2:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C436" s="16"/>
-    </row>
-    <row r="437" spans="2:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B437" s="19" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="438" spans="2:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B438" s="5" t="s">
-        <v>358</v>
-      </c>
-    </row>
-    <row r="439" spans="2:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B439" s="5" t="s">
-        <v>359</v>
-      </c>
-    </row>
-    <row r="440" spans="2:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B440" s="5" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="441" spans="2:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B441" s="5" t="s">
-        <v>360</v>
-      </c>
+    <row r="440" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B440" s="3"/>
+    </row>
+    <row r="441" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B441" s="19"/>
+    </row>
+    <row r="446" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B446" s="19"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -3752,169 +3789,173 @@
     <hyperlink ref="B208" r:id="rId162" xr:uid="{00000000-0004-0000-0000-0000A3000000}"/>
     <hyperlink ref="B209" r:id="rId163" xr:uid="{00000000-0004-0000-0000-0000A4000000}"/>
     <hyperlink ref="B210" r:id="rId164" xr:uid="{00000000-0004-0000-0000-0000A5000000}"/>
-    <hyperlink ref="B211" r:id="rId165" xr:uid="{00000000-0004-0000-0000-0000A6000000}"/>
-    <hyperlink ref="B214" r:id="rId166" xr:uid="{00000000-0004-0000-0000-0000A7000000}"/>
-    <hyperlink ref="B215" r:id="rId167" xr:uid="{00000000-0004-0000-0000-0000A8000000}"/>
-    <hyperlink ref="B216" r:id="rId168" xr:uid="{00000000-0004-0000-0000-0000A9000000}"/>
-    <hyperlink ref="B217" r:id="rId169" xr:uid="{00000000-0004-0000-0000-0000AA000000}"/>
-    <hyperlink ref="B218" r:id="rId170" xr:uid="{00000000-0004-0000-0000-0000AB000000}"/>
-    <hyperlink ref="B219" r:id="rId171" xr:uid="{00000000-0004-0000-0000-0000AC000000}"/>
-    <hyperlink ref="B220" r:id="rId172" xr:uid="{00000000-0004-0000-0000-0000AD000000}"/>
-    <hyperlink ref="B221" r:id="rId173" xr:uid="{00000000-0004-0000-0000-0000AE000000}"/>
-    <hyperlink ref="B222" r:id="rId174" xr:uid="{00000000-0004-0000-0000-0000AF000000}"/>
-    <hyperlink ref="B223" r:id="rId175" xr:uid="{00000000-0004-0000-0000-0000B0000000}"/>
-    <hyperlink ref="B224" r:id="rId176" xr:uid="{00000000-0004-0000-0000-0000B1000000}"/>
-    <hyperlink ref="B225" r:id="rId177" xr:uid="{00000000-0004-0000-0000-0000B2000000}"/>
-    <hyperlink ref="B226" r:id="rId178" xr:uid="{00000000-0004-0000-0000-0000B3000000}"/>
-    <hyperlink ref="B227" r:id="rId179" xr:uid="{00000000-0004-0000-0000-0000B4000000}"/>
-    <hyperlink ref="B228" r:id="rId180" xr:uid="{00000000-0004-0000-0000-0000B5000000}"/>
-    <hyperlink ref="B229" r:id="rId181" xr:uid="{00000000-0004-0000-0000-0000B6000000}"/>
-    <hyperlink ref="B230" r:id="rId182" xr:uid="{00000000-0004-0000-0000-0000B7000000}"/>
-    <hyperlink ref="B231" r:id="rId183" xr:uid="{00000000-0004-0000-0000-0000B8000000}"/>
-    <hyperlink ref="B234" r:id="rId184" xr:uid="{00000000-0004-0000-0000-0000B9000000}"/>
-    <hyperlink ref="B235" r:id="rId185" xr:uid="{00000000-0004-0000-0000-0000BA000000}"/>
-    <hyperlink ref="B236" r:id="rId186" xr:uid="{00000000-0004-0000-0000-0000BB000000}"/>
-    <hyperlink ref="B237" r:id="rId187" xr:uid="{00000000-0004-0000-0000-0000BC000000}"/>
-    <hyperlink ref="B238" r:id="rId188" xr:uid="{00000000-0004-0000-0000-0000BD000000}"/>
-    <hyperlink ref="B239" r:id="rId189" xr:uid="{00000000-0004-0000-0000-0000BE000000}"/>
-    <hyperlink ref="B240" r:id="rId190" xr:uid="{00000000-0004-0000-0000-0000BF000000}"/>
-    <hyperlink ref="B244" r:id="rId191" xr:uid="{00000000-0004-0000-0000-0000C0000000}"/>
-    <hyperlink ref="B245" r:id="rId192" xr:uid="{00000000-0004-0000-0000-0000C1000000}"/>
-    <hyperlink ref="B248" r:id="rId193" xr:uid="{00000000-0004-0000-0000-0000C2000000}"/>
-    <hyperlink ref="B249" r:id="rId194" xr:uid="{00000000-0004-0000-0000-0000C3000000}"/>
-    <hyperlink ref="B253" r:id="rId195" xr:uid="{00000000-0004-0000-0000-0000C4000000}"/>
-    <hyperlink ref="B254" r:id="rId196" xr:uid="{00000000-0004-0000-0000-0000C5000000}"/>
-    <hyperlink ref="B255" r:id="rId197" xr:uid="{00000000-0004-0000-0000-0000C6000000}"/>
-    <hyperlink ref="B256" r:id="rId198" xr:uid="{00000000-0004-0000-0000-0000C7000000}"/>
-    <hyperlink ref="B259" r:id="rId199" xr:uid="{00000000-0004-0000-0000-0000C8000000}"/>
-    <hyperlink ref="B260" r:id="rId200" xr:uid="{00000000-0004-0000-0000-0000C9000000}"/>
-    <hyperlink ref="B261" r:id="rId201" xr:uid="{00000000-0004-0000-0000-0000CA000000}"/>
-    <hyperlink ref="B262" r:id="rId202" xr:uid="{00000000-0004-0000-0000-0000CB000000}"/>
-    <hyperlink ref="B263" r:id="rId203" xr:uid="{00000000-0004-0000-0000-0000CC000000}"/>
-    <hyperlink ref="B264" r:id="rId204" xr:uid="{00000000-0004-0000-0000-0000CD000000}"/>
-    <hyperlink ref="B265" r:id="rId205" xr:uid="{00000000-0004-0000-0000-0000CE000000}"/>
-    <hyperlink ref="B266" r:id="rId206" xr:uid="{00000000-0004-0000-0000-0000CF000000}"/>
-    <hyperlink ref="B267" r:id="rId207" xr:uid="{00000000-0004-0000-0000-0000D0000000}"/>
-    <hyperlink ref="B270" r:id="rId208" xr:uid="{00000000-0004-0000-0000-0000D1000000}"/>
-    <hyperlink ref="B271" r:id="rId209" xr:uid="{00000000-0004-0000-0000-0000D2000000}"/>
-    <hyperlink ref="B272" r:id="rId210" xr:uid="{00000000-0004-0000-0000-0000D3000000}"/>
-    <hyperlink ref="B273" r:id="rId211" xr:uid="{00000000-0004-0000-0000-0000D4000000}"/>
-    <hyperlink ref="B274" r:id="rId212" xr:uid="{00000000-0004-0000-0000-0000D5000000}"/>
-    <hyperlink ref="B278" r:id="rId213" xr:uid="{00000000-0004-0000-0000-0000D6000000}"/>
-    <hyperlink ref="B279" r:id="rId214" xr:uid="{00000000-0004-0000-0000-0000D7000000}"/>
-    <hyperlink ref="B280" r:id="rId215" xr:uid="{00000000-0004-0000-0000-0000D8000000}"/>
-    <hyperlink ref="B281" r:id="rId216" xr:uid="{00000000-0004-0000-0000-0000D9000000}"/>
-    <hyperlink ref="B282" r:id="rId217" xr:uid="{00000000-0004-0000-0000-0000DA000000}"/>
-    <hyperlink ref="B285" r:id="rId218" xr:uid="{00000000-0004-0000-0000-0000DB000000}"/>
-    <hyperlink ref="B286" r:id="rId219" xr:uid="{00000000-0004-0000-0000-0000DC000000}"/>
-    <hyperlink ref="B287" r:id="rId220" xr:uid="{00000000-0004-0000-0000-0000DD000000}"/>
-    <hyperlink ref="B288" r:id="rId221" xr:uid="{00000000-0004-0000-0000-0000DE000000}"/>
-    <hyperlink ref="B292" r:id="rId222" xr:uid="{00000000-0004-0000-0000-0000DF000000}"/>
-    <hyperlink ref="B293" r:id="rId223" xr:uid="{00000000-0004-0000-0000-0000E0000000}"/>
-    <hyperlink ref="B294" r:id="rId224" xr:uid="{00000000-0004-0000-0000-0000E1000000}"/>
-    <hyperlink ref="B295" r:id="rId225" xr:uid="{00000000-0004-0000-0000-0000E2000000}"/>
-    <hyperlink ref="B296" r:id="rId226" xr:uid="{00000000-0004-0000-0000-0000E3000000}"/>
-    <hyperlink ref="B300" r:id="rId227" xr:uid="{00000000-0004-0000-0000-0000E4000000}"/>
-    <hyperlink ref="B301" r:id="rId228" xr:uid="{00000000-0004-0000-0000-0000E5000000}"/>
-    <hyperlink ref="B302" r:id="rId229" xr:uid="{00000000-0004-0000-0000-0000E6000000}"/>
-    <hyperlink ref="B303" r:id="rId230" xr:uid="{00000000-0004-0000-0000-0000E7000000}"/>
-    <hyperlink ref="B304" r:id="rId231" xr:uid="{00000000-0004-0000-0000-0000E8000000}"/>
-    <hyperlink ref="B305" r:id="rId232" xr:uid="{00000000-0004-0000-0000-0000E9000000}"/>
-    <hyperlink ref="B308" r:id="rId233" xr:uid="{00000000-0004-0000-0000-0000EA000000}"/>
-    <hyperlink ref="B309" r:id="rId234" xr:uid="{00000000-0004-0000-0000-0000EB000000}"/>
-    <hyperlink ref="B310" r:id="rId235" xr:uid="{00000000-0004-0000-0000-0000EC000000}"/>
-    <hyperlink ref="B311" r:id="rId236" xr:uid="{00000000-0004-0000-0000-0000ED000000}"/>
-    <hyperlink ref="B315" r:id="rId237" xr:uid="{00000000-0004-0000-0000-0000EE000000}"/>
-    <hyperlink ref="B316" r:id="rId238" xr:uid="{00000000-0004-0000-0000-0000EF000000}"/>
-    <hyperlink ref="C316" r:id="rId239" xr:uid="{00000000-0004-0000-0000-0000F0000000}"/>
-    <hyperlink ref="B317" r:id="rId240" xr:uid="{00000000-0004-0000-0000-0000F1000000}"/>
-    <hyperlink ref="B318" r:id="rId241" xr:uid="{00000000-0004-0000-0000-0000F2000000}"/>
-    <hyperlink ref="C319" r:id="rId242" xr:uid="{00000000-0004-0000-0000-0000F3000000}"/>
-    <hyperlink ref="B320" r:id="rId243" xr:uid="{00000000-0004-0000-0000-0000F4000000}"/>
-    <hyperlink ref="B323" r:id="rId244" xr:uid="{00000000-0004-0000-0000-0000F5000000}"/>
-    <hyperlink ref="B324" r:id="rId245" xr:uid="{00000000-0004-0000-0000-0000F6000000}"/>
-    <hyperlink ref="B325" r:id="rId246" xr:uid="{00000000-0004-0000-0000-0000F7000000}"/>
-    <hyperlink ref="B326" r:id="rId247" xr:uid="{00000000-0004-0000-0000-0000F8000000}"/>
-    <hyperlink ref="B327" r:id="rId248" xr:uid="{00000000-0004-0000-0000-0000F9000000}"/>
-    <hyperlink ref="B328" r:id="rId249" xr:uid="{00000000-0004-0000-0000-0000FA000000}"/>
-    <hyperlink ref="C328" r:id="rId250" xr:uid="{00000000-0004-0000-0000-0000FB000000}"/>
-    <hyperlink ref="B329" r:id="rId251" xr:uid="{00000000-0004-0000-0000-0000FC000000}"/>
-    <hyperlink ref="B333" r:id="rId252" xr:uid="{00000000-0004-0000-0000-0000FD000000}"/>
-    <hyperlink ref="B334" r:id="rId253" xr:uid="{00000000-0004-0000-0000-0000FE000000}"/>
-    <hyperlink ref="B335" r:id="rId254" xr:uid="{00000000-0004-0000-0000-0000FF000000}"/>
-    <hyperlink ref="B336" r:id="rId255" xr:uid="{00000000-0004-0000-0000-000000010000}"/>
-    <hyperlink ref="B337" r:id="rId256" xr:uid="{00000000-0004-0000-0000-000001010000}"/>
-    <hyperlink ref="B338" r:id="rId257" xr:uid="{00000000-0004-0000-0000-000002010000}"/>
-    <hyperlink ref="B339" r:id="rId258" xr:uid="{00000000-0004-0000-0000-000003010000}"/>
-    <hyperlink ref="B343" r:id="rId259" xr:uid="{00000000-0004-0000-0000-000004010000}"/>
-    <hyperlink ref="B344" r:id="rId260" xr:uid="{00000000-0004-0000-0000-000005010000}"/>
-    <hyperlink ref="B347" r:id="rId261" xr:uid="{00000000-0004-0000-0000-000006010000}"/>
-    <hyperlink ref="B348" r:id="rId262" xr:uid="{00000000-0004-0000-0000-000007010000}"/>
-    <hyperlink ref="B349" r:id="rId263" xr:uid="{00000000-0004-0000-0000-000008010000}"/>
-    <hyperlink ref="B350" r:id="rId264" xr:uid="{00000000-0004-0000-0000-000009010000}"/>
-    <hyperlink ref="B351" r:id="rId265" xr:uid="{00000000-0004-0000-0000-00000A010000}"/>
-    <hyperlink ref="B352" r:id="rId266" xr:uid="{00000000-0004-0000-0000-00000B010000}"/>
-    <hyperlink ref="B353" r:id="rId267" xr:uid="{00000000-0004-0000-0000-00000C010000}"/>
-    <hyperlink ref="B354" r:id="rId268" xr:uid="{00000000-0004-0000-0000-00000D010000}"/>
-    <hyperlink ref="B355" r:id="rId269" xr:uid="{00000000-0004-0000-0000-00000E010000}"/>
-    <hyperlink ref="B356" r:id="rId270" xr:uid="{00000000-0004-0000-0000-00000F010000}"/>
-    <hyperlink ref="B357" r:id="rId271" xr:uid="{00000000-0004-0000-0000-000010010000}"/>
-    <hyperlink ref="B358" r:id="rId272" xr:uid="{00000000-0004-0000-0000-000011010000}"/>
-    <hyperlink ref="B359" r:id="rId273" xr:uid="{00000000-0004-0000-0000-000012010000}"/>
-    <hyperlink ref="B360" r:id="rId274" xr:uid="{00000000-0004-0000-0000-000013010000}"/>
-    <hyperlink ref="B363" r:id="rId275" xr:uid="{00000000-0004-0000-0000-000014010000}"/>
-    <hyperlink ref="B367" r:id="rId276" xr:uid="{00000000-0004-0000-0000-000015010000}"/>
-    <hyperlink ref="B368" r:id="rId277" xr:uid="{00000000-0004-0000-0000-000016010000}"/>
-    <hyperlink ref="B369" r:id="rId278" xr:uid="{00000000-0004-0000-0000-000017010000}"/>
-    <hyperlink ref="B370" r:id="rId279" xr:uid="{00000000-0004-0000-0000-000018010000}"/>
-    <hyperlink ref="B371" r:id="rId280" xr:uid="{00000000-0004-0000-0000-000019010000}"/>
-    <hyperlink ref="B372" r:id="rId281" xr:uid="{00000000-0004-0000-0000-00001A010000}"/>
-    <hyperlink ref="B373" r:id="rId282" xr:uid="{00000000-0004-0000-0000-00001B010000}"/>
-    <hyperlink ref="B374" r:id="rId283" xr:uid="{00000000-0004-0000-0000-00001C010000}"/>
-    <hyperlink ref="B375" r:id="rId284" xr:uid="{00000000-0004-0000-0000-00001D010000}"/>
-    <hyperlink ref="B376" r:id="rId285" xr:uid="{00000000-0004-0000-0000-00001E010000}"/>
-    <hyperlink ref="B379" r:id="rId286" xr:uid="{00000000-0004-0000-0000-00001F010000}"/>
-    <hyperlink ref="B380" r:id="rId287" xr:uid="{00000000-0004-0000-0000-000020010000}"/>
-    <hyperlink ref="B381" r:id="rId288" xr:uid="{00000000-0004-0000-0000-000021010000}"/>
-    <hyperlink ref="B382" r:id="rId289" xr:uid="{00000000-0004-0000-0000-000022010000}"/>
-    <hyperlink ref="B383" r:id="rId290" xr:uid="{00000000-0004-0000-0000-000023010000}"/>
-    <hyperlink ref="B384" r:id="rId291" xr:uid="{00000000-0004-0000-0000-000024010000}"/>
-    <hyperlink ref="B385" r:id="rId292" xr:uid="{00000000-0004-0000-0000-000025010000}"/>
-    <hyperlink ref="B386" r:id="rId293" xr:uid="{00000000-0004-0000-0000-000026010000}"/>
-    <hyperlink ref="B387" r:id="rId294" xr:uid="{00000000-0004-0000-0000-000027010000}"/>
-    <hyperlink ref="B388" r:id="rId295" xr:uid="{00000000-0004-0000-0000-000028010000}"/>
-    <hyperlink ref="B389" r:id="rId296" xr:uid="{00000000-0004-0000-0000-000029010000}"/>
-    <hyperlink ref="B390" r:id="rId297" xr:uid="{00000000-0004-0000-0000-00002A010000}"/>
-    <hyperlink ref="B391" r:id="rId298" xr:uid="{00000000-0004-0000-0000-00002B010000}"/>
-    <hyperlink ref="B394" r:id="rId299" xr:uid="{00000000-0004-0000-0000-00002C010000}"/>
-    <hyperlink ref="B395" r:id="rId300" xr:uid="{00000000-0004-0000-0000-00002D010000}"/>
-    <hyperlink ref="B399" r:id="rId301" xr:uid="{00000000-0004-0000-0000-00002E010000}"/>
-    <hyperlink ref="B400" r:id="rId302" xr:uid="{00000000-0004-0000-0000-00002F010000}"/>
-    <hyperlink ref="B401" r:id="rId303" xr:uid="{00000000-0004-0000-0000-000030010000}"/>
-    <hyperlink ref="B402" r:id="rId304" xr:uid="{00000000-0004-0000-0000-000031010000}"/>
-    <hyperlink ref="B403" r:id="rId305" xr:uid="{00000000-0004-0000-0000-000032010000}"/>
-    <hyperlink ref="B404" r:id="rId306" xr:uid="{00000000-0004-0000-0000-000033010000}"/>
-    <hyperlink ref="B405" r:id="rId307" xr:uid="{00000000-0004-0000-0000-000034010000}"/>
-    <hyperlink ref="B406" r:id="rId308" xr:uid="{00000000-0004-0000-0000-000035010000}"/>
-    <hyperlink ref="B409" r:id="rId309" xr:uid="{00000000-0004-0000-0000-000036010000}"/>
-    <hyperlink ref="B410" r:id="rId310" xr:uid="{00000000-0004-0000-0000-000037010000}"/>
-    <hyperlink ref="B411" r:id="rId311" xr:uid="{00000000-0004-0000-0000-000038010000}"/>
-    <hyperlink ref="B412" r:id="rId312" xr:uid="{00000000-0004-0000-0000-000039010000}"/>
-    <hyperlink ref="B413" r:id="rId313" xr:uid="{00000000-0004-0000-0000-00003A010000}"/>
-    <hyperlink ref="B414" r:id="rId314" xr:uid="{00000000-0004-0000-0000-00003B010000}"/>
-    <hyperlink ref="B415" r:id="rId315" xr:uid="{00000000-0004-0000-0000-00003C010000}"/>
-    <hyperlink ref="B416" r:id="rId316" xr:uid="{00000000-0004-0000-0000-00003D010000}"/>
-    <hyperlink ref="B417" r:id="rId317" xr:uid="{00000000-0004-0000-0000-00003E010000}"/>
-    <hyperlink ref="B421" r:id="rId318" xr:uid="{00000000-0004-0000-0000-00003F010000}"/>
-    <hyperlink ref="B422" r:id="rId319" xr:uid="{00000000-0004-0000-0000-000040010000}"/>
-    <hyperlink ref="B423" r:id="rId320" xr:uid="{00000000-0004-0000-0000-000041010000}"/>
-    <hyperlink ref="B424" r:id="rId321" xr:uid="{00000000-0004-0000-0000-000042010000}"/>
-    <hyperlink ref="B427" r:id="rId322" xr:uid="{00000000-0004-0000-0000-000043010000}"/>
-    <hyperlink ref="B429" r:id="rId323" xr:uid="{00000000-0004-0000-0000-000044010000}"/>
-    <hyperlink ref="B433" r:id="rId324" xr:uid="{74B2161E-06D4-4B8A-9584-0E2CBADC274E}"/>
-    <hyperlink ref="B435" r:id="rId325" xr:uid="{1608CB90-B10C-47C4-93D4-59AEE1446147}"/>
+    <hyperlink ref="B221" r:id="rId165" xr:uid="{00000000-0004-0000-0000-0000A9000000}"/>
+    <hyperlink ref="B222" r:id="rId166" xr:uid="{00000000-0004-0000-0000-0000AA000000}"/>
+    <hyperlink ref="B223" r:id="rId167" xr:uid="{00000000-0004-0000-0000-0000AB000000}"/>
+    <hyperlink ref="B224" r:id="rId168" xr:uid="{00000000-0004-0000-0000-0000AC000000}"/>
+    <hyperlink ref="B225" r:id="rId169" xr:uid="{00000000-0004-0000-0000-0000AD000000}"/>
+    <hyperlink ref="B226" r:id="rId170" xr:uid="{00000000-0004-0000-0000-0000AE000000}"/>
+    <hyperlink ref="B227" r:id="rId171" xr:uid="{00000000-0004-0000-0000-0000AF000000}"/>
+    <hyperlink ref="B228" r:id="rId172" xr:uid="{00000000-0004-0000-0000-0000B0000000}"/>
+    <hyperlink ref="B229" r:id="rId173" xr:uid="{00000000-0004-0000-0000-0000B1000000}"/>
+    <hyperlink ref="B230" r:id="rId174" xr:uid="{00000000-0004-0000-0000-0000B2000000}"/>
+    <hyperlink ref="B231" r:id="rId175" xr:uid="{00000000-0004-0000-0000-0000B3000000}"/>
+    <hyperlink ref="B232" r:id="rId176" xr:uid="{00000000-0004-0000-0000-0000B4000000}"/>
+    <hyperlink ref="B233" r:id="rId177" xr:uid="{00000000-0004-0000-0000-0000B5000000}"/>
+    <hyperlink ref="B234" r:id="rId178" xr:uid="{00000000-0004-0000-0000-0000B6000000}"/>
+    <hyperlink ref="B235" r:id="rId179" xr:uid="{00000000-0004-0000-0000-0000B7000000}"/>
+    <hyperlink ref="B236" r:id="rId180" xr:uid="{00000000-0004-0000-0000-0000B8000000}"/>
+    <hyperlink ref="B243" r:id="rId181" xr:uid="{00000000-0004-0000-0000-0000B9000000}"/>
+    <hyperlink ref="B244" r:id="rId182" xr:uid="{00000000-0004-0000-0000-0000BA000000}"/>
+    <hyperlink ref="B245" r:id="rId183" xr:uid="{00000000-0004-0000-0000-0000BB000000}"/>
+    <hyperlink ref="B246" r:id="rId184" xr:uid="{00000000-0004-0000-0000-0000BC000000}"/>
+    <hyperlink ref="B247" r:id="rId185" xr:uid="{00000000-0004-0000-0000-0000BD000000}"/>
+    <hyperlink ref="B248" r:id="rId186" xr:uid="{00000000-0004-0000-0000-0000BE000000}"/>
+    <hyperlink ref="B249" r:id="rId187" xr:uid="{00000000-0004-0000-0000-0000BF000000}"/>
+    <hyperlink ref="B253" r:id="rId188" xr:uid="{00000000-0004-0000-0000-0000C0000000}"/>
+    <hyperlink ref="B254" r:id="rId189" xr:uid="{00000000-0004-0000-0000-0000C1000000}"/>
+    <hyperlink ref="B257" r:id="rId190" xr:uid="{00000000-0004-0000-0000-0000C2000000}"/>
+    <hyperlink ref="B258" r:id="rId191" xr:uid="{00000000-0004-0000-0000-0000C3000000}"/>
+    <hyperlink ref="B262" r:id="rId192" xr:uid="{00000000-0004-0000-0000-0000C4000000}"/>
+    <hyperlink ref="B263" r:id="rId193" xr:uid="{00000000-0004-0000-0000-0000C5000000}"/>
+    <hyperlink ref="B264" r:id="rId194" xr:uid="{00000000-0004-0000-0000-0000C6000000}"/>
+    <hyperlink ref="B265" r:id="rId195" xr:uid="{00000000-0004-0000-0000-0000C7000000}"/>
+    <hyperlink ref="B268" r:id="rId196" xr:uid="{00000000-0004-0000-0000-0000C8000000}"/>
+    <hyperlink ref="B269" r:id="rId197" xr:uid="{00000000-0004-0000-0000-0000C9000000}"/>
+    <hyperlink ref="B270" r:id="rId198" xr:uid="{00000000-0004-0000-0000-0000CA000000}"/>
+    <hyperlink ref="B271" r:id="rId199" xr:uid="{00000000-0004-0000-0000-0000CB000000}"/>
+    <hyperlink ref="B272" r:id="rId200" xr:uid="{00000000-0004-0000-0000-0000CC000000}"/>
+    <hyperlink ref="B273" r:id="rId201" xr:uid="{00000000-0004-0000-0000-0000CD000000}"/>
+    <hyperlink ref="B274" r:id="rId202" xr:uid="{00000000-0004-0000-0000-0000CE000000}"/>
+    <hyperlink ref="B275" r:id="rId203" xr:uid="{00000000-0004-0000-0000-0000CF000000}"/>
+    <hyperlink ref="B276" r:id="rId204" xr:uid="{00000000-0004-0000-0000-0000D0000000}"/>
+    <hyperlink ref="B279" r:id="rId205" xr:uid="{00000000-0004-0000-0000-0000D1000000}"/>
+    <hyperlink ref="B280" r:id="rId206" xr:uid="{00000000-0004-0000-0000-0000D2000000}"/>
+    <hyperlink ref="B281" r:id="rId207" xr:uid="{00000000-0004-0000-0000-0000D3000000}"/>
+    <hyperlink ref="B282" r:id="rId208" xr:uid="{00000000-0004-0000-0000-0000D4000000}"/>
+    <hyperlink ref="B283" r:id="rId209" xr:uid="{00000000-0004-0000-0000-0000D5000000}"/>
+    <hyperlink ref="B287" r:id="rId210" xr:uid="{00000000-0004-0000-0000-0000D6000000}"/>
+    <hyperlink ref="B288" r:id="rId211" xr:uid="{00000000-0004-0000-0000-0000D7000000}"/>
+    <hyperlink ref="B289" r:id="rId212" xr:uid="{00000000-0004-0000-0000-0000D8000000}"/>
+    <hyperlink ref="B290" r:id="rId213" xr:uid="{00000000-0004-0000-0000-0000D9000000}"/>
+    <hyperlink ref="B291" r:id="rId214" xr:uid="{00000000-0004-0000-0000-0000DA000000}"/>
+    <hyperlink ref="B294" r:id="rId215" xr:uid="{00000000-0004-0000-0000-0000DB000000}"/>
+    <hyperlink ref="B295" r:id="rId216" xr:uid="{00000000-0004-0000-0000-0000DC000000}"/>
+    <hyperlink ref="B296" r:id="rId217" xr:uid="{00000000-0004-0000-0000-0000DD000000}"/>
+    <hyperlink ref="B297" r:id="rId218" xr:uid="{00000000-0004-0000-0000-0000DE000000}"/>
+    <hyperlink ref="B301" r:id="rId219" xr:uid="{00000000-0004-0000-0000-0000DF000000}"/>
+    <hyperlink ref="B302" r:id="rId220" xr:uid="{00000000-0004-0000-0000-0000E0000000}"/>
+    <hyperlink ref="B303" r:id="rId221" xr:uid="{00000000-0004-0000-0000-0000E1000000}"/>
+    <hyperlink ref="B304" r:id="rId222" xr:uid="{00000000-0004-0000-0000-0000E2000000}"/>
+    <hyperlink ref="B305" r:id="rId223" xr:uid="{00000000-0004-0000-0000-0000E3000000}"/>
+    <hyperlink ref="B309" r:id="rId224" xr:uid="{00000000-0004-0000-0000-0000E4000000}"/>
+    <hyperlink ref="B310" r:id="rId225" xr:uid="{00000000-0004-0000-0000-0000E5000000}"/>
+    <hyperlink ref="B311" r:id="rId226" xr:uid="{00000000-0004-0000-0000-0000E6000000}"/>
+    <hyperlink ref="B312" r:id="rId227" xr:uid="{00000000-0004-0000-0000-0000E7000000}"/>
+    <hyperlink ref="B313" r:id="rId228" xr:uid="{00000000-0004-0000-0000-0000E8000000}"/>
+    <hyperlink ref="B314" r:id="rId229" xr:uid="{00000000-0004-0000-0000-0000E9000000}"/>
+    <hyperlink ref="B317" r:id="rId230" xr:uid="{00000000-0004-0000-0000-0000EA000000}"/>
+    <hyperlink ref="B318" r:id="rId231" xr:uid="{00000000-0004-0000-0000-0000EB000000}"/>
+    <hyperlink ref="B319" r:id="rId232" xr:uid="{00000000-0004-0000-0000-0000EC000000}"/>
+    <hyperlink ref="B320" r:id="rId233" xr:uid="{00000000-0004-0000-0000-0000ED000000}"/>
+    <hyperlink ref="B324" r:id="rId234" xr:uid="{00000000-0004-0000-0000-0000EE000000}"/>
+    <hyperlink ref="B325" r:id="rId235" xr:uid="{00000000-0004-0000-0000-0000EF000000}"/>
+    <hyperlink ref="C325" r:id="rId236" xr:uid="{00000000-0004-0000-0000-0000F0000000}"/>
+    <hyperlink ref="B326" r:id="rId237" xr:uid="{00000000-0004-0000-0000-0000F1000000}"/>
+    <hyperlink ref="B327" r:id="rId238" xr:uid="{00000000-0004-0000-0000-0000F2000000}"/>
+    <hyperlink ref="C328" r:id="rId239" xr:uid="{00000000-0004-0000-0000-0000F3000000}"/>
+    <hyperlink ref="B329" r:id="rId240" xr:uid="{00000000-0004-0000-0000-0000F4000000}"/>
+    <hyperlink ref="B332" r:id="rId241" xr:uid="{00000000-0004-0000-0000-0000F5000000}"/>
+    <hyperlink ref="B333" r:id="rId242" xr:uid="{00000000-0004-0000-0000-0000F6000000}"/>
+    <hyperlink ref="B334" r:id="rId243" xr:uid="{00000000-0004-0000-0000-0000F7000000}"/>
+    <hyperlink ref="B335" r:id="rId244" xr:uid="{00000000-0004-0000-0000-0000F8000000}"/>
+    <hyperlink ref="B336" r:id="rId245" xr:uid="{00000000-0004-0000-0000-0000F9000000}"/>
+    <hyperlink ref="B337" r:id="rId246" xr:uid="{00000000-0004-0000-0000-0000FA000000}"/>
+    <hyperlink ref="C337" r:id="rId247" xr:uid="{00000000-0004-0000-0000-0000FB000000}"/>
+    <hyperlink ref="B338" r:id="rId248" xr:uid="{00000000-0004-0000-0000-0000FC000000}"/>
+    <hyperlink ref="B342" r:id="rId249" xr:uid="{00000000-0004-0000-0000-0000FD000000}"/>
+    <hyperlink ref="B343" r:id="rId250" xr:uid="{00000000-0004-0000-0000-0000FE000000}"/>
+    <hyperlink ref="B344" r:id="rId251" xr:uid="{00000000-0004-0000-0000-0000FF000000}"/>
+    <hyperlink ref="B345" r:id="rId252" xr:uid="{00000000-0004-0000-0000-000000010000}"/>
+    <hyperlink ref="B346" r:id="rId253" xr:uid="{00000000-0004-0000-0000-000001010000}"/>
+    <hyperlink ref="B347" r:id="rId254" xr:uid="{00000000-0004-0000-0000-000002010000}"/>
+    <hyperlink ref="B348" r:id="rId255" xr:uid="{00000000-0004-0000-0000-000003010000}"/>
+    <hyperlink ref="B352" r:id="rId256" xr:uid="{00000000-0004-0000-0000-000004010000}"/>
+    <hyperlink ref="B353" r:id="rId257" xr:uid="{00000000-0004-0000-0000-000005010000}"/>
+    <hyperlink ref="B356" r:id="rId258" xr:uid="{00000000-0004-0000-0000-000006010000}"/>
+    <hyperlink ref="B357" r:id="rId259" xr:uid="{00000000-0004-0000-0000-000007010000}"/>
+    <hyperlink ref="B358" r:id="rId260" xr:uid="{00000000-0004-0000-0000-000008010000}"/>
+    <hyperlink ref="B359" r:id="rId261" xr:uid="{00000000-0004-0000-0000-000009010000}"/>
+    <hyperlink ref="B360" r:id="rId262" xr:uid="{00000000-0004-0000-0000-00000A010000}"/>
+    <hyperlink ref="B361" r:id="rId263" xr:uid="{00000000-0004-0000-0000-00000B010000}"/>
+    <hyperlink ref="B362" r:id="rId264" xr:uid="{00000000-0004-0000-0000-00000C010000}"/>
+    <hyperlink ref="B363" r:id="rId265" xr:uid="{00000000-0004-0000-0000-00000D010000}"/>
+    <hyperlink ref="B364" r:id="rId266" xr:uid="{00000000-0004-0000-0000-00000E010000}"/>
+    <hyperlink ref="B365" r:id="rId267" xr:uid="{00000000-0004-0000-0000-00000F010000}"/>
+    <hyperlink ref="B366" r:id="rId268" xr:uid="{00000000-0004-0000-0000-000010010000}"/>
+    <hyperlink ref="B367" r:id="rId269" xr:uid="{00000000-0004-0000-0000-000011010000}"/>
+    <hyperlink ref="B368" r:id="rId270" xr:uid="{00000000-0004-0000-0000-000012010000}"/>
+    <hyperlink ref="B369" r:id="rId271" xr:uid="{00000000-0004-0000-0000-000013010000}"/>
+    <hyperlink ref="B372" r:id="rId272" xr:uid="{00000000-0004-0000-0000-000014010000}"/>
+    <hyperlink ref="B376" r:id="rId273" xr:uid="{00000000-0004-0000-0000-000015010000}"/>
+    <hyperlink ref="B377" r:id="rId274" xr:uid="{00000000-0004-0000-0000-000016010000}"/>
+    <hyperlink ref="B378" r:id="rId275" xr:uid="{00000000-0004-0000-0000-000017010000}"/>
+    <hyperlink ref="B379" r:id="rId276" xr:uid="{00000000-0004-0000-0000-000018010000}"/>
+    <hyperlink ref="B380" r:id="rId277" xr:uid="{00000000-0004-0000-0000-000019010000}"/>
+    <hyperlink ref="B381" r:id="rId278" xr:uid="{00000000-0004-0000-0000-00001A010000}"/>
+    <hyperlink ref="B382" r:id="rId279" xr:uid="{00000000-0004-0000-0000-00001B010000}"/>
+    <hyperlink ref="B383" r:id="rId280" xr:uid="{00000000-0004-0000-0000-00001C010000}"/>
+    <hyperlink ref="B384" r:id="rId281" xr:uid="{00000000-0004-0000-0000-00001D010000}"/>
+    <hyperlink ref="B385" r:id="rId282" xr:uid="{00000000-0004-0000-0000-00001E010000}"/>
+    <hyperlink ref="B388" r:id="rId283" xr:uid="{00000000-0004-0000-0000-00001F010000}"/>
+    <hyperlink ref="B389" r:id="rId284" xr:uid="{00000000-0004-0000-0000-000020010000}"/>
+    <hyperlink ref="B390" r:id="rId285" xr:uid="{00000000-0004-0000-0000-000021010000}"/>
+    <hyperlink ref="B391" r:id="rId286" xr:uid="{00000000-0004-0000-0000-000022010000}"/>
+    <hyperlink ref="B392" r:id="rId287" xr:uid="{00000000-0004-0000-0000-000023010000}"/>
+    <hyperlink ref="B393" r:id="rId288" xr:uid="{00000000-0004-0000-0000-000024010000}"/>
+    <hyperlink ref="B394" r:id="rId289" xr:uid="{00000000-0004-0000-0000-000025010000}"/>
+    <hyperlink ref="B395" r:id="rId290" xr:uid="{00000000-0004-0000-0000-000026010000}"/>
+    <hyperlink ref="B396" r:id="rId291" xr:uid="{00000000-0004-0000-0000-000027010000}"/>
+    <hyperlink ref="B397" r:id="rId292" xr:uid="{00000000-0004-0000-0000-000028010000}"/>
+    <hyperlink ref="B398" r:id="rId293" xr:uid="{00000000-0004-0000-0000-000029010000}"/>
+    <hyperlink ref="B399" r:id="rId294" xr:uid="{00000000-0004-0000-0000-00002A010000}"/>
+    <hyperlink ref="B400" r:id="rId295" xr:uid="{00000000-0004-0000-0000-00002B010000}"/>
+    <hyperlink ref="B403" r:id="rId296" xr:uid="{00000000-0004-0000-0000-00002C010000}"/>
+    <hyperlink ref="B404" r:id="rId297" xr:uid="{00000000-0004-0000-0000-00002D010000}"/>
+    <hyperlink ref="B408" r:id="rId298" xr:uid="{00000000-0004-0000-0000-00002E010000}"/>
+    <hyperlink ref="B409" r:id="rId299" xr:uid="{00000000-0004-0000-0000-00002F010000}"/>
+    <hyperlink ref="B410" r:id="rId300" xr:uid="{00000000-0004-0000-0000-000030010000}"/>
+    <hyperlink ref="B411" r:id="rId301" xr:uid="{00000000-0004-0000-0000-000031010000}"/>
+    <hyperlink ref="B412" r:id="rId302" xr:uid="{00000000-0004-0000-0000-000032010000}"/>
+    <hyperlink ref="B413" r:id="rId303" xr:uid="{00000000-0004-0000-0000-000033010000}"/>
+    <hyperlink ref="B414" r:id="rId304" xr:uid="{00000000-0004-0000-0000-000034010000}"/>
+    <hyperlink ref="B415" r:id="rId305" xr:uid="{00000000-0004-0000-0000-000035010000}"/>
+    <hyperlink ref="B418" r:id="rId306" xr:uid="{00000000-0004-0000-0000-000036010000}"/>
+    <hyperlink ref="B419" r:id="rId307" xr:uid="{00000000-0004-0000-0000-000037010000}"/>
+    <hyperlink ref="B420" r:id="rId308" xr:uid="{00000000-0004-0000-0000-000038010000}"/>
+    <hyperlink ref="B421" r:id="rId309" xr:uid="{00000000-0004-0000-0000-000039010000}"/>
+    <hyperlink ref="B422" r:id="rId310" xr:uid="{00000000-0004-0000-0000-00003A010000}"/>
+    <hyperlink ref="B423" r:id="rId311" xr:uid="{00000000-0004-0000-0000-00003B010000}"/>
+    <hyperlink ref="B424" r:id="rId312" xr:uid="{00000000-0004-0000-0000-00003C010000}"/>
+    <hyperlink ref="B425" r:id="rId313" xr:uid="{00000000-0004-0000-0000-00003D010000}"/>
+    <hyperlink ref="B426" r:id="rId314" xr:uid="{00000000-0004-0000-0000-00003E010000}"/>
+    <hyperlink ref="B430" r:id="rId315" xr:uid="{00000000-0004-0000-0000-00003F010000}"/>
+    <hyperlink ref="B431" r:id="rId316" xr:uid="{00000000-0004-0000-0000-000040010000}"/>
+    <hyperlink ref="B432" r:id="rId317" xr:uid="{00000000-0004-0000-0000-000041010000}"/>
+    <hyperlink ref="B433" r:id="rId318" xr:uid="{00000000-0004-0000-0000-000042010000}"/>
+    <hyperlink ref="B436" r:id="rId319" xr:uid="{00000000-0004-0000-0000-000043010000}"/>
+    <hyperlink ref="B438" r:id="rId320" xr:uid="{00000000-0004-0000-0000-000044010000}"/>
+    <hyperlink ref="B212" r:id="rId321" xr:uid="{74B2161E-06D4-4B8A-9584-0E2CBADC274E}"/>
+    <hyperlink ref="B214" r:id="rId322" xr:uid="{1608CB90-B10C-47C4-93D4-59AEE1446147}"/>
+    <hyperlink ref="B237" r:id="rId323" xr:uid="{968F4BF9-FCA3-411D-B359-F57C0021CF6D}"/>
+    <hyperlink ref="B238" r:id="rId324" xr:uid="{3F6B4E87-4E97-43A0-926D-9BFAA64415F9}"/>
+    <hyperlink ref="B239" r:id="rId325" xr:uid="{06E52597-6E05-40D9-8554-1823C19D12DF}"/>
+    <hyperlink ref="B240" r:id="rId326" xr:uid="{986E706F-2DF0-485D-8DFF-AAF7D9593A61}"/>
+    <hyperlink ref="B211" r:id="rId327" xr:uid="{00000000-0004-0000-0000-0000A6000000}"/>
+    <hyperlink ref="B219" r:id="rId328" xr:uid="{00000000-0004-0000-0000-0000A7000000}"/>
+    <hyperlink ref="B220" r:id="rId329" xr:uid="{00000000-0004-0000-0000-0000A8000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId326"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId330"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
floor ceil and other problem
</commit_message>
<xml_diff>
--- a/DSA Sheet.xlsx
+++ b/DSA Sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d8cfd04c6706e178/Desktop/myDSA/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="89" documentId="11_3A057C0BE92A3E6736330E251CF58AC5C01E7902" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2312B033-161E-4749-8F78-DD8B061AF450}"/>
+  <xr:revisionPtr revIDLastSave="102" documentId="11_3A057C0BE92A3E6736330E251CF58AC5C01E7902" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{97BA890B-712B-4509-8AEF-44A5AF94AE3E}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="415" uniqueCount="376">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="420" uniqueCount="381">
   <si>
     <t>Arrays</t>
   </si>
@@ -1214,6 +1214,21 @@
   </si>
   <si>
     <t>can do but we need a little bit of understanding of mountains</t>
+  </si>
+  <si>
+    <t>take care of the edge cases</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/single-element-in-a-sorted-array/</t>
+  </si>
+  <si>
+    <t>a very good question on limits</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/search-insert-position/</t>
+  </si>
+  <si>
+    <t>I used recursion here, how to implement binary search</t>
   </si>
 </sst>
 </file>
@@ -1424,7 +1439,7 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="17" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="18" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="18" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="18" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1646,8 +1661,8 @@
   </sheetPr>
   <dimension ref="A1:D455"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A255" zoomScale="94" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D288" sqref="D288"/>
+    <sheetView tabSelected="1" topLeftCell="A258" zoomScale="94" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C279" sqref="C279"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2920,7 +2935,11 @@
         <v>375</v>
       </c>
     </row>
-    <row r="269" spans="2:3" ht="13.2" x14ac:dyDescent="0.25"/>
+    <row r="269" spans="2:3" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B269" s="22" t="s">
+        <v>379</v>
+      </c>
+    </row>
     <row r="270" spans="2:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B270" s="6"/>
     </row>
@@ -2955,8 +2974,11 @@
       </c>
     </row>
     <row r="277" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B277" s="6" t="s">
+      <c r="B277" s="14" t="s">
         <v>213</v>
+      </c>
+      <c r="C277" t="s">
+        <v>380</v>
       </c>
     </row>
     <row r="278" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
@@ -2965,8 +2987,11 @@
       </c>
     </row>
     <row r="279" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B279" s="6" t="s">
+      <c r="B279" s="22" t="s">
         <v>215</v>
+      </c>
+      <c r="C279" t="s">
+        <v>376</v>
       </c>
     </row>
     <row r="280" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2990,12 +3015,17 @@
       </c>
     </row>
     <row r="284" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B284" s="14" t="s">
+      <c r="B284" s="17" t="s">
         <v>371</v>
       </c>
     </row>
     <row r="285" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B285" s="6"/>
+      <c r="B285" s="21" t="s">
+        <v>377</v>
+      </c>
+      <c r="C285" t="s">
+        <v>378</v>
+      </c>
     </row>
     <row r="286" spans="1:3" ht="13.2" x14ac:dyDescent="0.25"/>
     <row r="287" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
@@ -4084,8 +4114,10 @@
     <hyperlink ref="B207" r:id="rId328" xr:uid="{4F5D2989-A407-4666-9C15-2E56FFB04CB9}"/>
     <hyperlink ref="B278" r:id="rId329" xr:uid="{75AF2DA5-CF21-4E60-9996-AB053317FCD9}"/>
     <hyperlink ref="B275" r:id="rId330" xr:uid="{78371077-6F60-4589-9248-A2A0CC2BB6FF}"/>
+    <hyperlink ref="B284" r:id="rId331" xr:uid="{551F7908-8ED4-4567-ACB7-9587817B333B}"/>
+    <hyperlink ref="B285" r:id="rId332" xr:uid="{8D443D6C-2BB4-4B14-98C0-8DB9BF3A33C1}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId331"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId333"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
learned a bit more questions
</commit_message>
<xml_diff>
--- a/DSA Sheet.xlsx
+++ b/DSA Sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d8cfd04c6706e178/Desktop/myDSA/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="102" documentId="11_3A057C0BE92A3E6736330E251CF58AC5C01E7902" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{97BA890B-712B-4509-8AEF-44A5AF94AE3E}"/>
+  <xr:revisionPtr revIDLastSave="108" documentId="11_3A057C0BE92A3E6736330E251CF58AC5C01E7902" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DC530647-9E92-4A3F-9E9D-AA8BB235B5A4}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="420" uniqueCount="381">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="421" uniqueCount="382">
   <si>
     <t>Arrays</t>
   </si>
@@ -1230,12 +1230,15 @@
   <si>
     <t>I used recursion here, how to implement binary search</t>
   </si>
+  <si>
+    <t>https://leetcode.com/problems/find-smallest-letter-greater-than-target/</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -1354,6 +1357,13 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color rgb="FF0070C0"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="6">
     <fill>
@@ -1400,7 +1410,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1440,6 +1450,7 @@
     <xf numFmtId="0" fontId="17" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="18" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="18" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="19" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1661,8 +1672,8 @@
   </sheetPr>
   <dimension ref="A1:D455"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A258" zoomScale="94" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C279" sqref="C279"/>
+    <sheetView tabSelected="1" topLeftCell="B258" zoomScale="105" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C286" sqref="C286"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2941,7 +2952,9 @@
       </c>
     </row>
     <row r="270" spans="2:3" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B270" s="6"/>
+      <c r="B270" s="29" t="s">
+        <v>381</v>
+      </c>
     </row>
     <row r="271" spans="2:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B271" s="6"/>
@@ -3020,7 +3033,7 @@
       </c>
     </row>
     <row r="285" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B285" s="21" t="s">
+      <c r="B285" s="17" t="s">
         <v>377</v>
       </c>
       <c r="C285" t="s">

</xml_diff>

<commit_message>
added questions from BS
</commit_message>
<xml_diff>
--- a/DSA Sheet.xlsx
+++ b/DSA Sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d8cfd04c6706e178/Desktop/myDSA/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="108" documentId="11_3A057C0BE92A3E6736330E251CF58AC5C01E7902" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DC530647-9E92-4A3F-9E9D-AA8BB235B5A4}"/>
+  <xr:revisionPtr revIDLastSave="124" documentId="11_3A057C0BE92A3E6736330E251CF58AC5C01E7902" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{40C2EAD7-48E5-4C5F-B8D1-216DADFF7DC5}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="421" uniqueCount="382">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="426" uniqueCount="387">
   <si>
     <t>Arrays</t>
   </si>
@@ -1233,12 +1233,27 @@
   <si>
     <t>https://leetcode.com/problems/find-smallest-letter-greater-than-target/</t>
   </si>
+  <si>
+    <t>tricky question yet easy</t>
+  </si>
+  <si>
+    <t>don’t know which type of sum is this. To use - sliding window with deque or not</t>
+  </si>
+  <si>
+    <t>beautiful, watched the sol and solved it by myself very beautiful using bs, take in mind the number of operations for each number. And you are done</t>
+  </si>
+  <si>
+    <t>we implement binary search tree</t>
+  </si>
+  <si>
+    <t>I will have to try this again this question is awesome</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="20" x14ac:knownFonts="1">
+  <fonts count="23" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -1364,6 +1379,26 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="4"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="4" tint="-0.499984740745262"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="6">
     <fill>
@@ -1410,7 +1445,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1449,8 +1484,10 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="17" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="18" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="18" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="19" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="20" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="22" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="21" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1672,8 +1709,8 @@
   </sheetPr>
   <dimension ref="A1:D455"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B258" zoomScale="105" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C286" sqref="C286"/>
+    <sheetView tabSelected="1" topLeftCell="A259" zoomScale="81" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B275" sqref="B275"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2934,12 +2971,15 @@
       </c>
     </row>
     <row r="267" spans="2:3" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B267" s="6" t="s">
+      <c r="B267" s="26" t="s">
         <v>209</v>
       </c>
+      <c r="C267" s="25" t="s">
+        <v>382</v>
+      </c>
     </row>
     <row r="268" spans="2:3" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B268" s="28" t="s">
+      <c r="B268" s="26" t="s">
         <v>210</v>
       </c>
       <c r="C268" s="25" t="s">
@@ -2952,7 +2992,7 @@
       </c>
     </row>
     <row r="270" spans="2:3" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B270" s="29" t="s">
+      <c r="B270" s="28" t="s">
         <v>381</v>
       </c>
     </row>
@@ -3008,7 +3048,7 @@
       </c>
     </row>
     <row r="280" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B280" s="6" t="s">
+      <c r="B280" s="29" t="s">
         <v>216</v>
       </c>
     </row>
@@ -3018,13 +3058,16 @@
       </c>
     </row>
     <row r="282" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B282" s="6" t="s">
+      <c r="B282" s="22" t="s">
         <v>218</v>
       </c>
     </row>
     <row r="283" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B283" s="6" t="s">
+      <c r="B283" s="14" t="s">
         <v>219</v>
+      </c>
+      <c r="C283" s="25" t="s">
+        <v>384</v>
       </c>
     </row>
     <row r="284" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
@@ -3047,78 +3090,87 @@
       </c>
     </row>
     <row r="288" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B288" s="6" t="s">
+      <c r="B288" s="14" t="s">
         <v>220</v>
       </c>
-    </row>
-    <row r="289" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B289" s="6" t="s">
+      <c r="C288" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="289" spans="2:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B289" s="31" t="s">
         <v>221</v>
       </c>
-    </row>
-    <row r="290" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="C289" s="25" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="290" spans="2:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B290" s="6" t="s">
         <v>222</v>
       </c>
     </row>
-    <row r="291" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B291" s="6" t="s">
+    <row r="291" spans="2:3" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B291" s="22" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="292" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B292" s="6" t="s">
+    <row r="292" spans="2:3" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B292" s="30" t="s">
         <v>224</v>
       </c>
-    </row>
-    <row r="293" spans="2:2" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="294" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="C292" s="25" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="293" spans="2:3" ht="13.2" x14ac:dyDescent="0.25"/>
+    <row r="294" spans="2:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B294" s="3" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="295" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="295" spans="2:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B295" s="4" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="296" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="296" spans="2:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B296" s="6" t="s">
         <v>226</v>
       </c>
     </row>
-    <row r="297" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="297" spans="2:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B297" s="6" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="298" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="298" spans="2:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B298" s="6" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="299" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="299" spans="2:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B299" s="6" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="300" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="300" spans="2:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B300" s="5" t="s">
         <v>230</v>
       </c>
     </row>
-    <row r="301" spans="2:2" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="302" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="301" spans="2:3" ht="13.2" x14ac:dyDescent="0.25"/>
+    <row r="302" spans="2:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B302" s="4" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="303" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="303" spans="2:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B303" s="6" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="304" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="304" spans="2:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B304" s="6" t="s">
         <v>232</v>
       </c>

</xml_diff>

<commit_message>
starting again so pushed
</commit_message>
<xml_diff>
--- a/DSA Sheet.xlsx
+++ b/DSA Sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d8cfd04c6706e178/Desktop/myDSA/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="113" documentId="13_ncr:1_{CCE37EA7-A2E4-4FF7-9902-EC3DA1D988F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{09209D8B-D465-4C40-8311-0FAE6B38A146}"/>
+  <xr:revisionPtr revIDLastSave="125" documentId="13_ncr:1_{CCE37EA7-A2E4-4FF7-9902-EC3DA1D988F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{42B5CA54-4923-4D7E-BBEC-7F6B19DBCB2A}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="490" uniqueCount="445">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="493" uniqueCount="448">
   <si>
     <t>Arrays</t>
   </si>
@@ -1421,6 +1421,15 @@
   </si>
   <si>
     <t>using hashmap nd dfs --- imp as tobe done by own</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/deepest-leaves-sum/</t>
+  </si>
+  <si>
+    <t>using level order traversal</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/find-a-corresponding-node-of-a-binary-tree-in-a-clone-of-that-tree/</t>
   </si>
 </sst>
 </file>
@@ -1625,7 +1634,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1681,6 +1690,7 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="21" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="17" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1900,10 +1910,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:D509"/>
+  <dimension ref="A1:D511"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A392" zoomScale="111" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C399" sqref="C399"/>
+      <selection activeCell="B407" sqref="B407"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3517,842 +3527,855 @@
         <v>14</v>
       </c>
     </row>
-    <row r="328" spans="2:3" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B328" s="6" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="329" spans="2:3" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B329" s="6" t="s">
-        <v>227</v>
+    <row r="328" spans="2:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B328" s="22" t="s">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="329" spans="2:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B329" s="22" t="s">
+        <v>445</v>
+      </c>
+      <c r="C329" s="25" t="s">
+        <v>446</v>
       </c>
     </row>
     <row r="330" spans="2:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B330" s="6" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
     </row>
     <row r="331" spans="2:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B331" s="6" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="332" spans="2:3" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B332" s="6" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="333" spans="2:3" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B333" s="6" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="332" spans="2:3" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B332" s="5" t="s">
+    <row r="334" spans="2:3" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B334" s="5" t="s">
         <v>230</v>
       </c>
     </row>
-    <row r="333" spans="2:3" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="334" spans="2:3" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B334" s="4" t="s">
+    <row r="335" spans="2:3" ht="13.2" x14ac:dyDescent="0.25"/>
+    <row r="336" spans="2:3" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B336" s="4" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="335" spans="2:3" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B335" s="6" t="s">
+    <row r="337" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B337" s="6" t="s">
         <v>231</v>
-      </c>
-    </row>
-    <row r="336" spans="2:3" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B336" s="6" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="337" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B337" s="6" t="s">
-        <v>233</v>
       </c>
     </row>
     <row r="338" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B338" s="6" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="339" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B339" s="6" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="340" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B340" s="6" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="339" spans="2:2" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="340" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B340" s="3" t="s">
+    <row r="341" spans="2:2" ht="13.2" x14ac:dyDescent="0.25"/>
+    <row r="342" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B342" s="3" t="s">
         <v>235</v>
       </c>
     </row>
-    <row r="341" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B341" s="4" t="s">
+    <row r="343" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B343" s="4" t="s">
         <v>236</v>
-      </c>
-    </row>
-    <row r="342" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B342" s="6" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="343" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B343" s="6" t="s">
-        <v>238</v>
       </c>
     </row>
     <row r="344" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B344" s="6" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="345" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="345" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B345" s="6" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
     </row>
     <row r="346" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B346" s="6" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="347" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B347" s="6" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="348" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B348" s="6" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="347" spans="2:2" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="348" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B348" s="3" t="s">
+    <row r="349" spans="2:2" ht="13.2" x14ac:dyDescent="0.25"/>
+    <row r="350" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B350" s="3" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="349" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B349" s="4" t="s">
+    <row r="351" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B351" s="4" t="s">
         <v>14</v>
-      </c>
-    </row>
-    <row r="350" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B350" s="6" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="351" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B351" s="6" t="s">
-        <v>244</v>
       </c>
     </row>
     <row r="352" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B352" s="6" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="353" spans="2:3" ht="13.2" x14ac:dyDescent="0.25">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="353" spans="2:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B353" s="6" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
     </row>
     <row r="354" spans="2:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B354" s="6" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="355" spans="2:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B355" s="6" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="356" spans="2:3" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B356" s="6" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="357" spans="2:3" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B357" s="6" t="s">
         <v>248</v>
       </c>
     </row>
-    <row r="356" spans="2:3" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="357" spans="2:3" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B357" s="4" t="s">
+    <row r="358" spans="2:3" ht="13.2" x14ac:dyDescent="0.25"/>
+    <row r="359" spans="2:3" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B359" s="4" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="358" spans="2:3" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B358" s="5" t="s">
+    <row r="360" spans="2:3" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B360" s="5" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="359" spans="2:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B359" s="6" t="s">
+    <row r="361" spans="2:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B361" s="6" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="360" spans="2:3" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B360" s="6" t="s">
+    <row r="362" spans="2:3" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B362" s="6" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="361" spans="2:3" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B361" s="6" t="s">
+    <row r="363" spans="2:3" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B363" s="6" t="s">
         <v>252</v>
       </c>
     </row>
-    <row r="362" spans="2:3" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="363" spans="2:3" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B363" s="3" t="s">
+    <row r="364" spans="2:3" ht="13.2" x14ac:dyDescent="0.25"/>
+    <row r="365" spans="2:3" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B365" s="3" t="s">
         <v>253</v>
       </c>
     </row>
-    <row r="364" spans="2:3" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B364" s="4" t="s">
+    <row r="366" spans="2:3" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B366" s="4" t="s">
         <v>1</v>
-      </c>
-    </row>
-    <row r="365" spans="2:3" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B365" s="6" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="366" spans="2:3" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B366" s="6" t="s">
-        <v>255</v>
-      </c>
-      <c r="C366" s="5" t="s">
-        <v>256</v>
       </c>
     </row>
     <row r="367" spans="2:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B367" s="6" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="368" spans="2:3" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B368" s="6" t="s">
+        <v>255</v>
+      </c>
+      <c r="C368" s="5" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="369" spans="2:3" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B369" s="6" t="s">
         <v>257</v>
       </c>
     </row>
-    <row r="368" spans="2:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B368" s="5" t="s">
+    <row r="370" spans="2:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B370" s="5" t="s">
         <v>258</v>
       </c>
     </row>
-    <row r="369" spans="2:3" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B369" s="20" t="s">
+    <row r="371" spans="2:3" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B371" s="20" t="s">
         <v>259</v>
       </c>
-      <c r="C369" s="8" t="s">
+      <c r="C371" s="8" t="s">
         <v>260</v>
       </c>
     </row>
-    <row r="370" spans="2:3" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B370" s="5" t="s">
+    <row r="372" spans="2:3" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B372" s="5" t="s">
         <v>261</v>
       </c>
     </row>
-    <row r="371" spans="2:3" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="372" spans="2:3" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B372" s="4" t="s">
+    <row r="373" spans="2:3" ht="13.2" x14ac:dyDescent="0.25"/>
+    <row r="374" spans="2:3" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B374" s="4" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="373" spans="2:3" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B373" s="5" t="s">
+    <row r="375" spans="2:3" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B375" s="5" t="s">
         <v>262</v>
       </c>
     </row>
-    <row r="374" spans="2:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B374" s="6" t="s">
+    <row r="376" spans="2:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B376" s="6" t="s">
         <v>263</v>
       </c>
     </row>
-    <row r="375" spans="2:3" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B375" s="6" t="s">
+    <row r="377" spans="2:3" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B377" s="6" t="s">
         <v>264</v>
-      </c>
-    </row>
-    <row r="376" spans="2:3" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B376" s="6" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="377" spans="2:3" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B377" s="5" t="s">
-        <v>266</v>
       </c>
     </row>
     <row r="378" spans="2:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B378" s="6" t="s">
-        <v>267</v>
-      </c>
-      <c r="C378" s="6" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
     </row>
     <row r="379" spans="2:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B379" s="5" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="380" spans="2:3" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B380" s="6" t="s">
+        <v>267</v>
+      </c>
+      <c r="C380" s="6" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="381" spans="2:3" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B381" s="5" t="s">
         <v>269</v>
       </c>
     </row>
-    <row r="380" spans="2:3" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="381" spans="2:3" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B381" s="3" t="s">
+    <row r="382" spans="2:3" ht="13.2" x14ac:dyDescent="0.25"/>
+    <row r="383" spans="2:3" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B383" s="3" t="s">
         <v>270</v>
       </c>
     </row>
-    <row r="382" spans="2:3" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B382" s="4" t="s">
+    <row r="384" spans="2:3" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B384" s="4" t="s">
         <v>271</v>
       </c>
     </row>
-    <row r="383" spans="2:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B383" s="5" t="s">
+    <row r="385" spans="2:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B385" s="5" t="s">
         <v>272</v>
-      </c>
-    </row>
-    <row r="384" spans="2:3" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B384" s="6" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="385" spans="2:3" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B385" s="6" t="s">
-        <v>274</v>
       </c>
     </row>
     <row r="386" spans="2:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B386" s="6" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
     </row>
     <row r="387" spans="2:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B387" s="6" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
     </row>
     <row r="388" spans="2:3" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B388" s="5" t="s">
-        <v>277</v>
+      <c r="B388" s="6" t="s">
+        <v>275</v>
       </c>
     </row>
     <row r="389" spans="2:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B389" s="6" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="390" spans="2:3" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B390" s="5" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="391" spans="2:3" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B391" s="6" t="s">
         <v>278</v>
       </c>
     </row>
-    <row r="390" spans="2:3" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="391" spans="2:3" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B391" s="3" t="s">
+    <row r="392" spans="2:3" ht="13.2" x14ac:dyDescent="0.25"/>
+    <row r="393" spans="2:3" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B393" s="3" t="s">
         <v>279</v>
       </c>
     </row>
-    <row r="392" spans="2:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B392" s="4" t="s">
+    <row r="394" spans="2:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B394" s="4" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="393" spans="2:3" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B393" s="15" t="s">
+    <row r="395" spans="2:3" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B395" s="15" t="s">
         <v>280</v>
       </c>
-      <c r="C393" t="s">
+      <c r="C395" t="s">
         <v>443</v>
       </c>
     </row>
-    <row r="394" spans="2:3" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B394" s="22" t="s">
+    <row r="396" spans="2:3" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B396" s="22" t="s">
         <v>281</v>
       </c>
     </row>
-    <row r="395" spans="2:3" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B395" s="10"/>
-    </row>
-    <row r="396" spans="2:3" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B396" s="4" t="s">
+    <row r="397" spans="2:3" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B397" s="10"/>
+    </row>
+    <row r="398" spans="2:3" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B398" s="4" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="397" spans="2:3" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B397" s="44" t="s">
+    <row r="399" spans="2:3" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B399" s="44" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="398" spans="2:3" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B398" s="39" t="s">
+    <row r="400" spans="2:3" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B400" s="45" t="s">
         <v>193</v>
       </c>
-      <c r="C398" s="25" t="s">
+      <c r="C400" s="25" t="s">
         <v>444</v>
-      </c>
-    </row>
-    <row r="399" spans="2:3" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B399" s="6" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="400" spans="2:3" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B400" s="6" t="s">
-        <v>283</v>
       </c>
     </row>
     <row r="401" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B401" s="6" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
     </row>
     <row r="402" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B402" s="6" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
     </row>
     <row r="403" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B403" s="6" t="s">
-        <v>286</v>
-      </c>
-    </row>
-    <row r="404" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="404" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B404" s="6" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
     </row>
     <row r="405" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B405" s="6" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="406" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="406" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B406" s="6" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
     </row>
     <row r="407" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B407" s="6" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
     </row>
     <row r="408" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B408" s="6" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
     </row>
     <row r="409" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B409" s="6" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
     </row>
     <row r="410" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B410" s="5" t="s">
-        <v>293</v>
+      <c r="B410" s="6" t="s">
+        <v>291</v>
       </c>
     </row>
     <row r="411" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B411" s="6" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="412" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B412" s="5" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="413" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B413" s="6" t="s">
         <v>294</v>
       </c>
     </row>
-    <row r="412" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B412" s="6" t="s">
+    <row r="414" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B414" s="6" t="s">
         <v>295</v>
       </c>
     </row>
-    <row r="413" spans="2:2" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="414" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B414" s="3" t="s">
+    <row r="415" spans="2:2" ht="13.2" x14ac:dyDescent="0.25"/>
+    <row r="416" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B416" s="3" t="s">
         <v>296</v>
       </c>
     </row>
-    <row r="415" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B415" s="6" t="s">
+    <row r="417" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B417" s="6" t="s">
         <v>297</v>
       </c>
     </row>
-    <row r="416" spans="2:2" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="417" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B417" s="3" t="s">
+    <row r="418" spans="2:2" ht="13.2" x14ac:dyDescent="0.25"/>
+    <row r="419" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B419" s="3" t="s">
         <v>298</v>
       </c>
     </row>
-    <row r="418" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B418" s="11" t="s">
+    <row r="420" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B420" s="11" t="s">
         <v>1</v>
-      </c>
-    </row>
-    <row r="419" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B419" s="6" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="420" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B420" s="6" t="s">
-        <v>300</v>
       </c>
     </row>
     <row r="421" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B421" s="6" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
     </row>
     <row r="422" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B422" s="6" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
     </row>
     <row r="423" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B423" s="6" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
     </row>
     <row r="424" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B424" s="6" t="s">
-        <v>304</v>
-      </c>
-    </row>
-    <row r="425" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="425" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B425" s="6" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
     </row>
     <row r="426" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B426" s="6" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="427" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B427" s="6" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="428" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B428" s="6" t="s">
         <v>306</v>
       </c>
     </row>
-    <row r="427" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B427" s="6" t="s">
+    <row r="429" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B429" s="6" t="s">
         <v>307</v>
       </c>
     </row>
-    <row r="428" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B428" s="6" t="s">
+    <row r="430" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B430" s="6" t="s">
         <v>308</v>
       </c>
     </row>
-    <row r="429" spans="2:2" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="430" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B430" s="4" t="s">
+    <row r="431" spans="2:2" ht="13.2" x14ac:dyDescent="0.25"/>
+    <row r="432" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B432" s="4" t="s">
         <v>14</v>
-      </c>
-    </row>
-    <row r="431" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B431" s="6" t="s">
-        <v>309</v>
-      </c>
-    </row>
-    <row r="432" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B432" s="6" t="s">
-        <v>310</v>
       </c>
     </row>
     <row r="433" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B433" s="6" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
     </row>
     <row r="434" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B434" s="6" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="435" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B435" s="6" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="436" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B436" s="6" t="s">
         <v>312</v>
       </c>
     </row>
-    <row r="435" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B435" s="5" t="s">
+    <row r="437" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B437" s="5" t="s">
         <v>313</v>
-      </c>
-    </row>
-    <row r="436" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B436" s="5" t="s">
-        <v>314</v>
-      </c>
-    </row>
-    <row r="437" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B437" s="6" t="s">
-        <v>315</v>
       </c>
     </row>
     <row r="438" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B438" s="5" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
     </row>
     <row r="439" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B439" s="6" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="440" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B440" s="5" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="441" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B441" s="6" t="s">
         <v>317</v>
-      </c>
-    </row>
-    <row r="440" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B440" s="6" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="441" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B441" s="6" t="s">
-        <v>319</v>
       </c>
     </row>
     <row r="442" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B442" s="6" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="443" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B443" s="6" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="444" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B444" s="6" t="s">
         <v>320</v>
       </c>
     </row>
-    <row r="443" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B443" s="6" t="s">
+    <row r="445" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B445" s="6" t="s">
         <v>321</v>
       </c>
     </row>
-    <row r="444" spans="2:2" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="445" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B445" s="4" t="s">
+    <row r="446" spans="2:2" ht="13.2" x14ac:dyDescent="0.25"/>
+    <row r="447" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B447" s="4" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="446" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B446" s="5" t="s">
+    <row r="448" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B448" s="5" t="s">
         <v>322</v>
       </c>
     </row>
-    <row r="447" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B447" s="6" t="s">
+    <row r="449" spans="2:3" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B449" s="6" t="s">
         <v>323</v>
       </c>
     </row>
-    <row r="448" spans="2:2" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="449" spans="2:3" ht="13.2" x14ac:dyDescent="0.25"/>
     <row r="450" spans="2:3" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="451" spans="2:3" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B451" s="3" t="s">
+    <row r="451" spans="2:3" ht="13.2" x14ac:dyDescent="0.25"/>
+    <row r="452" spans="2:3" ht="13.2" x14ac:dyDescent="0.25"/>
+    <row r="453" spans="2:3" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B453" s="3" t="s">
         <v>324</v>
       </c>
     </row>
-    <row r="452" spans="2:3" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B452" s="3"/>
-    </row>
-    <row r="453" spans="2:3" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B453" s="4" t="s">
+    <row r="454" spans="2:3" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B454" s="3"/>
+    </row>
+    <row r="455" spans="2:3" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B455" s="4" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="454" spans="2:3" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B454" s="17" t="s">
+    <row r="456" spans="2:3" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B456" s="17" t="s">
         <v>429</v>
       </c>
-      <c r="C454" s="25" t="s">
+      <c r="C456" s="25" t="s">
         <v>430</v>
       </c>
     </row>
-    <row r="455" spans="2:3" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B455" s="17" t="s">
+    <row r="457" spans="2:3" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B457" s="17" t="s">
         <v>424</v>
       </c>
     </row>
-    <row r="456" spans="2:3" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B456" s="22" t="s">
+    <row r="458" spans="2:3" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B458" s="22" t="s">
         <v>427</v>
       </c>
-      <c r="C456" s="25" t="s">
+      <c r="C458" s="25" t="s">
         <v>428</v>
       </c>
     </row>
-    <row r="457" spans="2:3" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B457" s="22" t="s">
+    <row r="459" spans="2:3" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B459" s="22" t="s">
         <v>425</v>
       </c>
-      <c r="C457" s="25" t="s">
+      <c r="C459" s="25" t="s">
         <v>426</v>
       </c>
     </row>
-    <row r="458" spans="2:3" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B458" s="14" t="s">
+    <row r="460" spans="2:3" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B460" s="14" t="s">
         <v>433</v>
       </c>
-      <c r="C458" s="25" t="s">
+      <c r="C460" s="25" t="s">
         <v>434</v>
       </c>
     </row>
-    <row r="459" spans="2:3" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="460" spans="2:3" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="461" spans="2:3" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B461" s="4" t="s">
-        <v>14</v>
-      </c>
-    </row>
+    <row r="461" spans="2:3" ht="13.2" x14ac:dyDescent="0.25"/>
     <row r="462" spans="2:3" ht="13.2" x14ac:dyDescent="0.25"/>
     <row r="463" spans="2:3" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B463" s="22" t="s">
-        <v>204</v>
-      </c>
-      <c r="C463" t="s">
-        <v>432</v>
-      </c>
-    </row>
-    <row r="464" spans="2:3" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B464" s="22" t="s">
-        <v>325</v>
-      </c>
-    </row>
+      <c r="B463" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="464" spans="2:3" ht="13.2" x14ac:dyDescent="0.25"/>
     <row r="465" spans="2:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B465" s="22" t="s">
-        <v>326</v>
+        <v>204</v>
       </c>
       <c r="C465" t="s">
-        <v>423</v>
+        <v>432</v>
       </c>
     </row>
     <row r="466" spans="2:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B466" s="22" t="s">
-        <v>398</v>
+        <v>325</v>
       </c>
     </row>
     <row r="467" spans="2:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B467" s="22" t="s">
+        <v>326</v>
+      </c>
+      <c r="C467" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="468" spans="2:3" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B468" s="22" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="469" spans="2:3" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B469" s="22" t="s">
         <v>435</v>
-      </c>
-    </row>
-    <row r="468" spans="2:3" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B468" s="6" t="s">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="469" spans="2:3" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B469" s="6" t="s">
-        <v>328</v>
       </c>
     </row>
     <row r="470" spans="2:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B470" s="6" t="s">
-        <v>329</v>
-      </c>
-    </row>
-    <row r="471" spans="2:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="471" spans="2:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B471" s="6" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
     </row>
     <row r="472" spans="2:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B472" s="6" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="473" spans="2:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B473" s="6" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="474" spans="2:3" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B474" s="6" t="s">
         <v>331</v>
       </c>
     </row>
-    <row r="473" spans="2:3" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B473" s="6" t="s">
+    <row r="475" spans="2:3" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B475" s="6" t="s">
         <v>332</v>
       </c>
     </row>
-    <row r="474" spans="2:3" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B474" s="22" t="s">
+    <row r="476" spans="2:3" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B476" s="22" t="s">
         <v>431</v>
       </c>
     </row>
-    <row r="475" spans="2:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B475" s="4" t="s">
+    <row r="477" spans="2:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B477" s="4" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="476" spans="2:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B476" s="14" t="s">
+    <row r="478" spans="2:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B478" s="14" t="s">
         <v>441</v>
       </c>
-      <c r="C476" t="s">
+      <c r="C478" t="s">
         <v>442</v>
-      </c>
-    </row>
-    <row r="477" spans="2:3" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B477" s="6" t="s">
-        <v>322</v>
-      </c>
-    </row>
-    <row r="478" spans="2:3" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B478" s="6" t="s">
-        <v>333</v>
       </c>
     </row>
     <row r="479" spans="2:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B479" s="6" t="s">
-        <v>334</v>
+        <v>322</v>
       </c>
     </row>
     <row r="480" spans="2:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B480" s="6" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
     </row>
     <row r="481" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B481" s="5" t="s">
-        <v>336</v>
+      <c r="B481" s="6" t="s">
+        <v>334</v>
       </c>
     </row>
     <row r="482" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B482" s="6" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
     </row>
     <row r="483" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B483" s="6" t="s">
-        <v>338</v>
+      <c r="B483" s="5" t="s">
+        <v>336</v>
       </c>
     </row>
     <row r="484" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B484" s="6" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
     </row>
     <row r="485" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B485" s="6" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="486" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B486" s="6" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="487" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B487" s="6" t="s">
         <v>340</v>
       </c>
     </row>
-    <row r="486" spans="2:2" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="487" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B487" s="3" t="s">
+    <row r="488" spans="2:2" ht="13.2" x14ac:dyDescent="0.25"/>
+    <row r="489" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B489" s="3" t="s">
         <v>341</v>
       </c>
     </row>
-    <row r="488" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B488" s="4" t="s">
+    <row r="490" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B490" s="4" t="s">
         <v>342</v>
-      </c>
-    </row>
-    <row r="489" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B489" s="6" t="s">
-        <v>343</v>
-      </c>
-    </row>
-    <row r="490" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B490" s="6" t="s">
-        <v>344</v>
       </c>
     </row>
     <row r="491" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B491" s="6" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="492" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B492" s="6" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="493" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B493" s="6" t="s">
         <v>345</v>
       </c>
     </row>
-    <row r="492" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B492" s="12" t="s">
+    <row r="494" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B494" s="12" t="s">
         <v>346</v>
       </c>
     </row>
-    <row r="493" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B493" s="4"/>
-    </row>
-    <row r="494" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B494" s="3" t="s">
-        <v>347</v>
-      </c>
-    </row>
     <row r="495" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B495" s="5" t="s">
-        <v>348</v>
-      </c>
+      <c r="B495" s="4"/>
     </row>
     <row r="496" spans="2:2" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B496" s="3" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
     </row>
     <row r="497" spans="2:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B497" s="5" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="498" spans="2:3" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B498" s="3" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="499" spans="2:3" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B499" s="5" t="s">
         <v>350</v>
       </c>
     </row>
-    <row r="499" spans="2:3" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B499" s="3"/>
-    </row>
-    <row r="500" spans="2:3" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B500" s="19"/>
-    </row>
-    <row r="501" spans="2:3" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="502" spans="2:3" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="503" spans="2:3" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="C503" t="s">
+    <row r="501" spans="2:3" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B501" s="3"/>
+    </row>
+    <row r="502" spans="2:3" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B502" s="19"/>
+    </row>
+    <row r="503" spans="2:3" ht="13.2" x14ac:dyDescent="0.25"/>
+    <row r="504" spans="2:3" ht="13.2" x14ac:dyDescent="0.25"/>
+    <row r="505" spans="2:3" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="C505" t="s">
         <v>436</v>
       </c>
     </row>
-    <row r="504" spans="2:3" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B504" s="3" t="s">
+    <row r="506" spans="2:3" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B506" s="3" t="s">
         <v>437</v>
       </c>
     </row>
-    <row r="505" spans="2:3" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B505" s="19"/>
-    </row>
-    <row r="506" spans="2:3" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B506" s="42" t="s">
+    <row r="507" spans="2:3" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B507" s="19"/>
+    </row>
+    <row r="508" spans="2:3" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B508" s="42" t="s">
         <v>78</v>
       </c>
-      <c r="C506" t="s">
+      <c r="C508" t="s">
         <v>438</v>
       </c>
     </row>
-    <row r="507" spans="2:3" ht="13.2" x14ac:dyDescent="0.25"/>
-    <row r="508" spans="2:3" ht="13.2" x14ac:dyDescent="0.25"/>
     <row r="509" spans="2:3" ht="13.2" x14ac:dyDescent="0.25"/>
+    <row r="510" spans="2:3" ht="13.2" x14ac:dyDescent="0.25"/>
+    <row r="511" spans="2:3" ht="13.2" x14ac:dyDescent="0.25"/>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B7" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
@@ -4508,117 +4531,117 @@
     <hyperlink ref="B322" r:id="rId151" xr:uid="{00000000-0004-0000-0000-0000D3000000}"/>
     <hyperlink ref="B323" r:id="rId152" xr:uid="{00000000-0004-0000-0000-0000D4000000}"/>
     <hyperlink ref="B324" r:id="rId153" xr:uid="{00000000-0004-0000-0000-0000D5000000}"/>
-    <hyperlink ref="B328" r:id="rId154" xr:uid="{00000000-0004-0000-0000-0000D6000000}"/>
-    <hyperlink ref="B329" r:id="rId155" xr:uid="{00000000-0004-0000-0000-0000D7000000}"/>
-    <hyperlink ref="B330" r:id="rId156" xr:uid="{00000000-0004-0000-0000-0000D8000000}"/>
-    <hyperlink ref="B331" r:id="rId157" xr:uid="{00000000-0004-0000-0000-0000D9000000}"/>
-    <hyperlink ref="B332" r:id="rId158" xr:uid="{00000000-0004-0000-0000-0000DA000000}"/>
-    <hyperlink ref="B335" r:id="rId159" xr:uid="{00000000-0004-0000-0000-0000DB000000}"/>
-    <hyperlink ref="B336" r:id="rId160" xr:uid="{00000000-0004-0000-0000-0000DC000000}"/>
-    <hyperlink ref="B337" r:id="rId161" xr:uid="{00000000-0004-0000-0000-0000DD000000}"/>
-    <hyperlink ref="B338" r:id="rId162" xr:uid="{00000000-0004-0000-0000-0000DE000000}"/>
-    <hyperlink ref="B342" r:id="rId163" xr:uid="{00000000-0004-0000-0000-0000DF000000}"/>
-    <hyperlink ref="B343" r:id="rId164" xr:uid="{00000000-0004-0000-0000-0000E0000000}"/>
-    <hyperlink ref="B344" r:id="rId165" xr:uid="{00000000-0004-0000-0000-0000E1000000}"/>
-    <hyperlink ref="B345" r:id="rId166" xr:uid="{00000000-0004-0000-0000-0000E2000000}"/>
-    <hyperlink ref="B346" r:id="rId167" xr:uid="{00000000-0004-0000-0000-0000E3000000}"/>
-    <hyperlink ref="B350" r:id="rId168" xr:uid="{00000000-0004-0000-0000-0000E4000000}"/>
-    <hyperlink ref="B351" r:id="rId169" xr:uid="{00000000-0004-0000-0000-0000E5000000}"/>
-    <hyperlink ref="B352" r:id="rId170" xr:uid="{00000000-0004-0000-0000-0000E6000000}"/>
-    <hyperlink ref="B353" r:id="rId171" xr:uid="{00000000-0004-0000-0000-0000E7000000}"/>
-    <hyperlink ref="B354" r:id="rId172" xr:uid="{00000000-0004-0000-0000-0000E8000000}"/>
-    <hyperlink ref="B355" r:id="rId173" xr:uid="{00000000-0004-0000-0000-0000E9000000}"/>
-    <hyperlink ref="B358" r:id="rId174" xr:uid="{00000000-0004-0000-0000-0000EA000000}"/>
-    <hyperlink ref="B359" r:id="rId175" xr:uid="{00000000-0004-0000-0000-0000EB000000}"/>
-    <hyperlink ref="B360" r:id="rId176" xr:uid="{00000000-0004-0000-0000-0000EC000000}"/>
-    <hyperlink ref="B361" r:id="rId177" xr:uid="{00000000-0004-0000-0000-0000ED000000}"/>
-    <hyperlink ref="B365" r:id="rId178" xr:uid="{00000000-0004-0000-0000-0000EE000000}"/>
-    <hyperlink ref="B366" r:id="rId179" xr:uid="{00000000-0004-0000-0000-0000EF000000}"/>
-    <hyperlink ref="C366" r:id="rId180" xr:uid="{00000000-0004-0000-0000-0000F0000000}"/>
-    <hyperlink ref="B367" r:id="rId181" xr:uid="{00000000-0004-0000-0000-0000F1000000}"/>
-    <hyperlink ref="B368" r:id="rId182" xr:uid="{00000000-0004-0000-0000-0000F2000000}"/>
-    <hyperlink ref="C369" r:id="rId183" xr:uid="{00000000-0004-0000-0000-0000F3000000}"/>
-    <hyperlink ref="B370" r:id="rId184" xr:uid="{00000000-0004-0000-0000-0000F4000000}"/>
-    <hyperlink ref="B373" r:id="rId185" xr:uid="{00000000-0004-0000-0000-0000F5000000}"/>
-    <hyperlink ref="B374" r:id="rId186" xr:uid="{00000000-0004-0000-0000-0000F6000000}"/>
-    <hyperlink ref="B375" r:id="rId187" xr:uid="{00000000-0004-0000-0000-0000F7000000}"/>
-    <hyperlink ref="B376" r:id="rId188" xr:uid="{00000000-0004-0000-0000-0000F8000000}"/>
-    <hyperlink ref="B377" r:id="rId189" xr:uid="{00000000-0004-0000-0000-0000F9000000}"/>
-    <hyperlink ref="B378" r:id="rId190" xr:uid="{00000000-0004-0000-0000-0000FA000000}"/>
-    <hyperlink ref="C378" r:id="rId191" xr:uid="{00000000-0004-0000-0000-0000FB000000}"/>
-    <hyperlink ref="B379" r:id="rId192" xr:uid="{00000000-0004-0000-0000-0000FC000000}"/>
-    <hyperlink ref="B383" r:id="rId193" xr:uid="{00000000-0004-0000-0000-0000FD000000}"/>
-    <hyperlink ref="B384" r:id="rId194" xr:uid="{00000000-0004-0000-0000-0000FE000000}"/>
-    <hyperlink ref="B385" r:id="rId195" xr:uid="{00000000-0004-0000-0000-0000FF000000}"/>
-    <hyperlink ref="B386" r:id="rId196" xr:uid="{00000000-0004-0000-0000-000000010000}"/>
-    <hyperlink ref="B387" r:id="rId197" xr:uid="{00000000-0004-0000-0000-000001010000}"/>
-    <hyperlink ref="B388" r:id="rId198" xr:uid="{00000000-0004-0000-0000-000002010000}"/>
-    <hyperlink ref="B389" r:id="rId199" xr:uid="{00000000-0004-0000-0000-000003010000}"/>
-    <hyperlink ref="B393" r:id="rId200" xr:uid="{00000000-0004-0000-0000-000004010000}"/>
-    <hyperlink ref="B394" r:id="rId201" xr:uid="{00000000-0004-0000-0000-000005010000}"/>
-    <hyperlink ref="B399" r:id="rId202" xr:uid="{00000000-0004-0000-0000-000006010000}"/>
-    <hyperlink ref="B400" r:id="rId203" xr:uid="{00000000-0004-0000-0000-000007010000}"/>
-    <hyperlink ref="B401" r:id="rId204" xr:uid="{00000000-0004-0000-0000-000008010000}"/>
-    <hyperlink ref="B402" r:id="rId205" xr:uid="{00000000-0004-0000-0000-000009010000}"/>
-    <hyperlink ref="B403" r:id="rId206" xr:uid="{00000000-0004-0000-0000-00000A010000}"/>
-    <hyperlink ref="B404" r:id="rId207" xr:uid="{00000000-0004-0000-0000-00000B010000}"/>
-    <hyperlink ref="B405" r:id="rId208" xr:uid="{00000000-0004-0000-0000-00000C010000}"/>
-    <hyperlink ref="B406" r:id="rId209" xr:uid="{00000000-0004-0000-0000-00000D010000}"/>
-    <hyperlink ref="B407" r:id="rId210" xr:uid="{00000000-0004-0000-0000-00000E010000}"/>
-    <hyperlink ref="B408" r:id="rId211" xr:uid="{00000000-0004-0000-0000-00000F010000}"/>
-    <hyperlink ref="B409" r:id="rId212" xr:uid="{00000000-0004-0000-0000-000010010000}"/>
-    <hyperlink ref="B410" r:id="rId213" xr:uid="{00000000-0004-0000-0000-000011010000}"/>
-    <hyperlink ref="B411" r:id="rId214" xr:uid="{00000000-0004-0000-0000-000012010000}"/>
-    <hyperlink ref="B412" r:id="rId215" xr:uid="{00000000-0004-0000-0000-000013010000}"/>
-    <hyperlink ref="B415" r:id="rId216" xr:uid="{00000000-0004-0000-0000-000014010000}"/>
-    <hyperlink ref="B419" r:id="rId217" xr:uid="{00000000-0004-0000-0000-000015010000}"/>
-    <hyperlink ref="B420" r:id="rId218" xr:uid="{00000000-0004-0000-0000-000016010000}"/>
-    <hyperlink ref="B421" r:id="rId219" xr:uid="{00000000-0004-0000-0000-000017010000}"/>
-    <hyperlink ref="B422" r:id="rId220" xr:uid="{00000000-0004-0000-0000-000018010000}"/>
-    <hyperlink ref="B423" r:id="rId221" xr:uid="{00000000-0004-0000-0000-000019010000}"/>
-    <hyperlink ref="B424" r:id="rId222" xr:uid="{00000000-0004-0000-0000-00001A010000}"/>
-    <hyperlink ref="B425" r:id="rId223" xr:uid="{00000000-0004-0000-0000-00001B010000}"/>
-    <hyperlink ref="B426" r:id="rId224" xr:uid="{00000000-0004-0000-0000-00001C010000}"/>
-    <hyperlink ref="B427" r:id="rId225" xr:uid="{00000000-0004-0000-0000-00001D010000}"/>
-    <hyperlink ref="B428" r:id="rId226" xr:uid="{00000000-0004-0000-0000-00001E010000}"/>
-    <hyperlink ref="B431" r:id="rId227" xr:uid="{00000000-0004-0000-0000-00001F010000}"/>
-    <hyperlink ref="B432" r:id="rId228" xr:uid="{00000000-0004-0000-0000-000020010000}"/>
-    <hyperlink ref="B433" r:id="rId229" xr:uid="{00000000-0004-0000-0000-000021010000}"/>
-    <hyperlink ref="B434" r:id="rId230" xr:uid="{00000000-0004-0000-0000-000022010000}"/>
-    <hyperlink ref="B435" r:id="rId231" xr:uid="{00000000-0004-0000-0000-000023010000}"/>
-    <hyperlink ref="B436" r:id="rId232" xr:uid="{00000000-0004-0000-0000-000024010000}"/>
-    <hyperlink ref="B437" r:id="rId233" xr:uid="{00000000-0004-0000-0000-000025010000}"/>
-    <hyperlink ref="B438" r:id="rId234" xr:uid="{00000000-0004-0000-0000-000026010000}"/>
-    <hyperlink ref="B439" r:id="rId235" xr:uid="{00000000-0004-0000-0000-000027010000}"/>
-    <hyperlink ref="B440" r:id="rId236" xr:uid="{00000000-0004-0000-0000-000028010000}"/>
-    <hyperlink ref="B441" r:id="rId237" xr:uid="{00000000-0004-0000-0000-000029010000}"/>
-    <hyperlink ref="B442" r:id="rId238" xr:uid="{00000000-0004-0000-0000-00002A010000}"/>
-    <hyperlink ref="B443" r:id="rId239" xr:uid="{00000000-0004-0000-0000-00002B010000}"/>
-    <hyperlink ref="B446" r:id="rId240" xr:uid="{00000000-0004-0000-0000-00002C010000}"/>
-    <hyperlink ref="B447" r:id="rId241" xr:uid="{00000000-0004-0000-0000-00002D010000}"/>
-    <hyperlink ref="B464" r:id="rId242" xr:uid="{00000000-0004-0000-0000-00002E010000}"/>
-    <hyperlink ref="B465" r:id="rId243" xr:uid="{00000000-0004-0000-0000-00002F010000}"/>
-    <hyperlink ref="B468" r:id="rId244" xr:uid="{00000000-0004-0000-0000-000030010000}"/>
-    <hyperlink ref="B469" r:id="rId245" xr:uid="{00000000-0004-0000-0000-000031010000}"/>
-    <hyperlink ref="B470" r:id="rId246" xr:uid="{00000000-0004-0000-0000-000032010000}"/>
-    <hyperlink ref="B471" r:id="rId247" xr:uid="{00000000-0004-0000-0000-000033010000}"/>
-    <hyperlink ref="B472" r:id="rId248" xr:uid="{00000000-0004-0000-0000-000034010000}"/>
-    <hyperlink ref="B473" r:id="rId249" xr:uid="{00000000-0004-0000-0000-000035010000}"/>
-    <hyperlink ref="B477" r:id="rId250" xr:uid="{00000000-0004-0000-0000-000036010000}"/>
-    <hyperlink ref="B478" r:id="rId251" xr:uid="{00000000-0004-0000-0000-000037010000}"/>
-    <hyperlink ref="B479" r:id="rId252" xr:uid="{00000000-0004-0000-0000-000038010000}"/>
-    <hyperlink ref="B480" r:id="rId253" xr:uid="{00000000-0004-0000-0000-000039010000}"/>
-    <hyperlink ref="B481" r:id="rId254" xr:uid="{00000000-0004-0000-0000-00003A010000}"/>
-    <hyperlink ref="B482" r:id="rId255" xr:uid="{00000000-0004-0000-0000-00003B010000}"/>
-    <hyperlink ref="B483" r:id="rId256" xr:uid="{00000000-0004-0000-0000-00003C010000}"/>
-    <hyperlink ref="B484" r:id="rId257" xr:uid="{00000000-0004-0000-0000-00003D010000}"/>
-    <hyperlink ref="B485" r:id="rId258" xr:uid="{00000000-0004-0000-0000-00003E010000}"/>
-    <hyperlink ref="B489" r:id="rId259" xr:uid="{00000000-0004-0000-0000-00003F010000}"/>
-    <hyperlink ref="B490" r:id="rId260" xr:uid="{00000000-0004-0000-0000-000040010000}"/>
-    <hyperlink ref="B491" r:id="rId261" xr:uid="{00000000-0004-0000-0000-000041010000}"/>
-    <hyperlink ref="B492" r:id="rId262" xr:uid="{00000000-0004-0000-0000-000042010000}"/>
-    <hyperlink ref="B495" r:id="rId263" xr:uid="{00000000-0004-0000-0000-000043010000}"/>
-    <hyperlink ref="B497" r:id="rId264" xr:uid="{00000000-0004-0000-0000-000044010000}"/>
+    <hyperlink ref="B330" r:id="rId154" xr:uid="{00000000-0004-0000-0000-0000D6000000}"/>
+    <hyperlink ref="B331" r:id="rId155" xr:uid="{00000000-0004-0000-0000-0000D7000000}"/>
+    <hyperlink ref="B332" r:id="rId156" xr:uid="{00000000-0004-0000-0000-0000D8000000}"/>
+    <hyperlink ref="B333" r:id="rId157" xr:uid="{00000000-0004-0000-0000-0000D9000000}"/>
+    <hyperlink ref="B334" r:id="rId158" xr:uid="{00000000-0004-0000-0000-0000DA000000}"/>
+    <hyperlink ref="B337" r:id="rId159" xr:uid="{00000000-0004-0000-0000-0000DB000000}"/>
+    <hyperlink ref="B338" r:id="rId160" xr:uid="{00000000-0004-0000-0000-0000DC000000}"/>
+    <hyperlink ref="B339" r:id="rId161" xr:uid="{00000000-0004-0000-0000-0000DD000000}"/>
+    <hyperlink ref="B340" r:id="rId162" xr:uid="{00000000-0004-0000-0000-0000DE000000}"/>
+    <hyperlink ref="B344" r:id="rId163" xr:uid="{00000000-0004-0000-0000-0000DF000000}"/>
+    <hyperlink ref="B345" r:id="rId164" xr:uid="{00000000-0004-0000-0000-0000E0000000}"/>
+    <hyperlink ref="B346" r:id="rId165" xr:uid="{00000000-0004-0000-0000-0000E1000000}"/>
+    <hyperlink ref="B347" r:id="rId166" xr:uid="{00000000-0004-0000-0000-0000E2000000}"/>
+    <hyperlink ref="B348" r:id="rId167" xr:uid="{00000000-0004-0000-0000-0000E3000000}"/>
+    <hyperlink ref="B352" r:id="rId168" xr:uid="{00000000-0004-0000-0000-0000E4000000}"/>
+    <hyperlink ref="B353" r:id="rId169" xr:uid="{00000000-0004-0000-0000-0000E5000000}"/>
+    <hyperlink ref="B354" r:id="rId170" xr:uid="{00000000-0004-0000-0000-0000E6000000}"/>
+    <hyperlink ref="B355" r:id="rId171" xr:uid="{00000000-0004-0000-0000-0000E7000000}"/>
+    <hyperlink ref="B356" r:id="rId172" xr:uid="{00000000-0004-0000-0000-0000E8000000}"/>
+    <hyperlink ref="B357" r:id="rId173" xr:uid="{00000000-0004-0000-0000-0000E9000000}"/>
+    <hyperlink ref="B360" r:id="rId174" xr:uid="{00000000-0004-0000-0000-0000EA000000}"/>
+    <hyperlink ref="B361" r:id="rId175" xr:uid="{00000000-0004-0000-0000-0000EB000000}"/>
+    <hyperlink ref="B362" r:id="rId176" xr:uid="{00000000-0004-0000-0000-0000EC000000}"/>
+    <hyperlink ref="B363" r:id="rId177" xr:uid="{00000000-0004-0000-0000-0000ED000000}"/>
+    <hyperlink ref="B367" r:id="rId178" xr:uid="{00000000-0004-0000-0000-0000EE000000}"/>
+    <hyperlink ref="B368" r:id="rId179" xr:uid="{00000000-0004-0000-0000-0000EF000000}"/>
+    <hyperlink ref="C368" r:id="rId180" xr:uid="{00000000-0004-0000-0000-0000F0000000}"/>
+    <hyperlink ref="B369" r:id="rId181" xr:uid="{00000000-0004-0000-0000-0000F1000000}"/>
+    <hyperlink ref="B370" r:id="rId182" xr:uid="{00000000-0004-0000-0000-0000F2000000}"/>
+    <hyperlink ref="C371" r:id="rId183" xr:uid="{00000000-0004-0000-0000-0000F3000000}"/>
+    <hyperlink ref="B372" r:id="rId184" xr:uid="{00000000-0004-0000-0000-0000F4000000}"/>
+    <hyperlink ref="B375" r:id="rId185" xr:uid="{00000000-0004-0000-0000-0000F5000000}"/>
+    <hyperlink ref="B376" r:id="rId186" xr:uid="{00000000-0004-0000-0000-0000F6000000}"/>
+    <hyperlink ref="B377" r:id="rId187" xr:uid="{00000000-0004-0000-0000-0000F7000000}"/>
+    <hyperlink ref="B378" r:id="rId188" xr:uid="{00000000-0004-0000-0000-0000F8000000}"/>
+    <hyperlink ref="B379" r:id="rId189" xr:uid="{00000000-0004-0000-0000-0000F9000000}"/>
+    <hyperlink ref="B380" r:id="rId190" xr:uid="{00000000-0004-0000-0000-0000FA000000}"/>
+    <hyperlink ref="C380" r:id="rId191" xr:uid="{00000000-0004-0000-0000-0000FB000000}"/>
+    <hyperlink ref="B381" r:id="rId192" xr:uid="{00000000-0004-0000-0000-0000FC000000}"/>
+    <hyperlink ref="B385" r:id="rId193" xr:uid="{00000000-0004-0000-0000-0000FD000000}"/>
+    <hyperlink ref="B386" r:id="rId194" xr:uid="{00000000-0004-0000-0000-0000FE000000}"/>
+    <hyperlink ref="B387" r:id="rId195" xr:uid="{00000000-0004-0000-0000-0000FF000000}"/>
+    <hyperlink ref="B388" r:id="rId196" xr:uid="{00000000-0004-0000-0000-000000010000}"/>
+    <hyperlink ref="B389" r:id="rId197" xr:uid="{00000000-0004-0000-0000-000001010000}"/>
+    <hyperlink ref="B390" r:id="rId198" xr:uid="{00000000-0004-0000-0000-000002010000}"/>
+    <hyperlink ref="B391" r:id="rId199" xr:uid="{00000000-0004-0000-0000-000003010000}"/>
+    <hyperlink ref="B395" r:id="rId200" xr:uid="{00000000-0004-0000-0000-000004010000}"/>
+    <hyperlink ref="B396" r:id="rId201" xr:uid="{00000000-0004-0000-0000-000005010000}"/>
+    <hyperlink ref="B401" r:id="rId202" xr:uid="{00000000-0004-0000-0000-000006010000}"/>
+    <hyperlink ref="B402" r:id="rId203" xr:uid="{00000000-0004-0000-0000-000007010000}"/>
+    <hyperlink ref="B403" r:id="rId204" xr:uid="{00000000-0004-0000-0000-000008010000}"/>
+    <hyperlink ref="B404" r:id="rId205" xr:uid="{00000000-0004-0000-0000-000009010000}"/>
+    <hyperlink ref="B405" r:id="rId206" xr:uid="{00000000-0004-0000-0000-00000A010000}"/>
+    <hyperlink ref="B406" r:id="rId207" xr:uid="{00000000-0004-0000-0000-00000B010000}"/>
+    <hyperlink ref="B407" r:id="rId208" xr:uid="{00000000-0004-0000-0000-00000C010000}"/>
+    <hyperlink ref="B408" r:id="rId209" xr:uid="{00000000-0004-0000-0000-00000D010000}"/>
+    <hyperlink ref="B409" r:id="rId210" xr:uid="{00000000-0004-0000-0000-00000E010000}"/>
+    <hyperlink ref="B410" r:id="rId211" xr:uid="{00000000-0004-0000-0000-00000F010000}"/>
+    <hyperlink ref="B411" r:id="rId212" xr:uid="{00000000-0004-0000-0000-000010010000}"/>
+    <hyperlink ref="B412" r:id="rId213" xr:uid="{00000000-0004-0000-0000-000011010000}"/>
+    <hyperlink ref="B413" r:id="rId214" xr:uid="{00000000-0004-0000-0000-000012010000}"/>
+    <hyperlink ref="B414" r:id="rId215" xr:uid="{00000000-0004-0000-0000-000013010000}"/>
+    <hyperlink ref="B417" r:id="rId216" xr:uid="{00000000-0004-0000-0000-000014010000}"/>
+    <hyperlink ref="B421" r:id="rId217" xr:uid="{00000000-0004-0000-0000-000015010000}"/>
+    <hyperlink ref="B422" r:id="rId218" xr:uid="{00000000-0004-0000-0000-000016010000}"/>
+    <hyperlink ref="B423" r:id="rId219" xr:uid="{00000000-0004-0000-0000-000017010000}"/>
+    <hyperlink ref="B424" r:id="rId220" xr:uid="{00000000-0004-0000-0000-000018010000}"/>
+    <hyperlink ref="B425" r:id="rId221" xr:uid="{00000000-0004-0000-0000-000019010000}"/>
+    <hyperlink ref="B426" r:id="rId222" xr:uid="{00000000-0004-0000-0000-00001A010000}"/>
+    <hyperlink ref="B427" r:id="rId223" xr:uid="{00000000-0004-0000-0000-00001B010000}"/>
+    <hyperlink ref="B428" r:id="rId224" xr:uid="{00000000-0004-0000-0000-00001C010000}"/>
+    <hyperlink ref="B429" r:id="rId225" xr:uid="{00000000-0004-0000-0000-00001D010000}"/>
+    <hyperlink ref="B430" r:id="rId226" xr:uid="{00000000-0004-0000-0000-00001E010000}"/>
+    <hyperlink ref="B433" r:id="rId227" xr:uid="{00000000-0004-0000-0000-00001F010000}"/>
+    <hyperlink ref="B434" r:id="rId228" xr:uid="{00000000-0004-0000-0000-000020010000}"/>
+    <hyperlink ref="B435" r:id="rId229" xr:uid="{00000000-0004-0000-0000-000021010000}"/>
+    <hyperlink ref="B436" r:id="rId230" xr:uid="{00000000-0004-0000-0000-000022010000}"/>
+    <hyperlink ref="B437" r:id="rId231" xr:uid="{00000000-0004-0000-0000-000023010000}"/>
+    <hyperlink ref="B438" r:id="rId232" xr:uid="{00000000-0004-0000-0000-000024010000}"/>
+    <hyperlink ref="B439" r:id="rId233" xr:uid="{00000000-0004-0000-0000-000025010000}"/>
+    <hyperlink ref="B440" r:id="rId234" xr:uid="{00000000-0004-0000-0000-000026010000}"/>
+    <hyperlink ref="B441" r:id="rId235" xr:uid="{00000000-0004-0000-0000-000027010000}"/>
+    <hyperlink ref="B442" r:id="rId236" xr:uid="{00000000-0004-0000-0000-000028010000}"/>
+    <hyperlink ref="B443" r:id="rId237" xr:uid="{00000000-0004-0000-0000-000029010000}"/>
+    <hyperlink ref="B444" r:id="rId238" xr:uid="{00000000-0004-0000-0000-00002A010000}"/>
+    <hyperlink ref="B445" r:id="rId239" xr:uid="{00000000-0004-0000-0000-00002B010000}"/>
+    <hyperlink ref="B448" r:id="rId240" xr:uid="{00000000-0004-0000-0000-00002C010000}"/>
+    <hyperlink ref="B449" r:id="rId241" xr:uid="{00000000-0004-0000-0000-00002D010000}"/>
+    <hyperlink ref="B466" r:id="rId242" xr:uid="{00000000-0004-0000-0000-00002E010000}"/>
+    <hyperlink ref="B467" r:id="rId243" xr:uid="{00000000-0004-0000-0000-00002F010000}"/>
+    <hyperlink ref="B470" r:id="rId244" xr:uid="{00000000-0004-0000-0000-000030010000}"/>
+    <hyperlink ref="B471" r:id="rId245" xr:uid="{00000000-0004-0000-0000-000031010000}"/>
+    <hyperlink ref="B472" r:id="rId246" xr:uid="{00000000-0004-0000-0000-000032010000}"/>
+    <hyperlink ref="B473" r:id="rId247" xr:uid="{00000000-0004-0000-0000-000033010000}"/>
+    <hyperlink ref="B474" r:id="rId248" xr:uid="{00000000-0004-0000-0000-000034010000}"/>
+    <hyperlink ref="B475" r:id="rId249" xr:uid="{00000000-0004-0000-0000-000035010000}"/>
+    <hyperlink ref="B479" r:id="rId250" xr:uid="{00000000-0004-0000-0000-000036010000}"/>
+    <hyperlink ref="B480" r:id="rId251" xr:uid="{00000000-0004-0000-0000-000037010000}"/>
+    <hyperlink ref="B481" r:id="rId252" xr:uid="{00000000-0004-0000-0000-000038010000}"/>
+    <hyperlink ref="B482" r:id="rId253" xr:uid="{00000000-0004-0000-0000-000039010000}"/>
+    <hyperlink ref="B483" r:id="rId254" xr:uid="{00000000-0004-0000-0000-00003A010000}"/>
+    <hyperlink ref="B484" r:id="rId255" xr:uid="{00000000-0004-0000-0000-00003B010000}"/>
+    <hyperlink ref="B485" r:id="rId256" xr:uid="{00000000-0004-0000-0000-00003C010000}"/>
+    <hyperlink ref="B486" r:id="rId257" xr:uid="{00000000-0004-0000-0000-00003D010000}"/>
+    <hyperlink ref="B487" r:id="rId258" xr:uid="{00000000-0004-0000-0000-00003E010000}"/>
+    <hyperlink ref="B491" r:id="rId259" xr:uid="{00000000-0004-0000-0000-00003F010000}"/>
+    <hyperlink ref="B492" r:id="rId260" xr:uid="{00000000-0004-0000-0000-000040010000}"/>
+    <hyperlink ref="B493" r:id="rId261" xr:uid="{00000000-0004-0000-0000-000041010000}"/>
+    <hyperlink ref="B494" r:id="rId262" xr:uid="{00000000-0004-0000-0000-000042010000}"/>
+    <hyperlink ref="B497" r:id="rId263" xr:uid="{00000000-0004-0000-0000-000043010000}"/>
+    <hyperlink ref="B499" r:id="rId264" xr:uid="{00000000-0004-0000-0000-000044010000}"/>
     <hyperlink ref="B244" r:id="rId265" xr:uid="{74B2161E-06D4-4B8A-9584-0E2CBADC274E}"/>
     <hyperlink ref="B246" r:id="rId266" xr:uid="{1608CB90-B10C-47C4-93D4-59AEE1446147}"/>
     <hyperlink ref="B270" r:id="rId267" xr:uid="{968F4BF9-FCA3-411D-B359-F57C0021CF6D}"/>
@@ -4695,9 +4718,9 @@
     <hyperlink ref="B81" r:id="rId338" xr:uid="{8ED0000A-50AE-4CD4-8333-C135BC7CAA86}"/>
     <hyperlink ref="B86" r:id="rId339" xr:uid="{EB551A3E-779F-43F1-BE5F-BE3382AB3ADF}"/>
     <hyperlink ref="B63" r:id="rId340" xr:uid="{74A357C6-1996-40A9-A1A0-8F4FFC6F43DA}"/>
-    <hyperlink ref="B455" r:id="rId341" xr:uid="{884B8A48-BF54-453B-AFD0-71384A8E4670}"/>
-    <hyperlink ref="B506" r:id="rId342" xr:uid="{632C56C6-AA7B-4927-8DC4-7D17ED02C3C2}"/>
-    <hyperlink ref="B398" r:id="rId343" xr:uid="{7F79710E-6CD7-4EF6-9A80-B8578C230F1B}"/>
+    <hyperlink ref="B457" r:id="rId341" xr:uid="{884B8A48-BF54-453B-AFD0-71384A8E4670}"/>
+    <hyperlink ref="B508" r:id="rId342" xr:uid="{632C56C6-AA7B-4927-8DC4-7D17ED02C3C2}"/>
+    <hyperlink ref="B400" r:id="rId343" xr:uid="{7F79710E-6CD7-4EF6-9A80-B8578C230F1B}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId344"/>

</xml_diff>